<commit_message>
Added y1918 into R and removed cities/rural districts from y1918 on excel, so only total deaths remained.
</commit_message>
<xml_diff>
--- a/CA 1900-2020 Project.xlsx
+++ b/CA 1900-2020 Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCB3DD2-EE5E-A544-8654-AE5DEA52F034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9510D0A-84DB-1948-B04A-62198A076083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y1900" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9564" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9562" uniqueCount="1289">
   <si>
     <t>Notes</t>
   </si>
@@ -42543,26 +42543,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5E015A-69B3-E449-BA8B-148C187E74C0}">
-  <dimension ref="A1:J206"/>
+  <dimension ref="A1:H206"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="50.83203125" style="48" customWidth="1"/>
     <col min="3" max="5" width="25.83203125" style="48" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="48"/>
-    <col min="7" max="7" width="11.83203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="48" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="48"/>
-    <col min="10" max="10" width="14.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="48"/>
+    <col min="6" max="6" width="10.83203125" style="48" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="48"/>
+    <col min="8" max="8" width="14.6640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="171" t="s">
         <v>60</v>
       </c>
@@ -42578,24 +42576,18 @@
       <c r="E1" s="127" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="31" t="s">
-        <v>894</v>
-      </c>
-      <c r="G1" s="158" t="s">
-        <v>895</v>
-      </c>
-      <c r="H1" s="155" t="s">
+      <c r="F1" s="155" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="48">
-        <f>SUM(H2:H205)</f>
+      <c r="G1" s="48">
+        <f>SUM(F2:F205)</f>
         <v>56488</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="H1" s="48" t="s">
         <v>1235</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>507</v>
       </c>
@@ -42612,17 +42604,10 @@
         <v>89</v>
       </c>
       <c r="F2" s="33">
-        <v>99</v>
-      </c>
-      <c r="G2" s="48">
-        <v>97</v>
-      </c>
-      <c r="H2" s="33">
-        <f>F2+G2</f>
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="33" t="s">
         <v>509</v>
       </c>
@@ -42635,13 +42620,11 @@
       <c r="E3" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="H3" s="33">
-        <f t="shared" ref="H3:H66" si="0">F3+G3</f>
+      <c r="F3" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="33" t="s">
         <v>510</v>
       </c>
@@ -42654,13 +42637,11 @@
       <c r="E4" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="H4" s="33">
-        <f t="shared" si="0"/>
+      <c r="F4" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
         <v>146</v>
       </c>
@@ -42674,17 +42655,10 @@
         <v>89</v>
       </c>
       <c r="F5" s="33">
-        <v>12</v>
-      </c>
-      <c r="G5" s="48">
-        <v>29</v>
-      </c>
-      <c r="H5" s="33">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="33" t="s">
         <v>140</v>
       </c>
@@ -42698,17 +42672,10 @@
         <v>89</v>
       </c>
       <c r="F6" s="33">
-        <v>1</v>
-      </c>
-      <c r="G6" s="48">
-        <v>2</v>
-      </c>
-      <c r="H6" s="33">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="33" t="s">
         <v>141</v>
       </c>
@@ -42722,17 +42689,10 @@
         <v>89</v>
       </c>
       <c r="F7" s="33">
-        <v>69</v>
-      </c>
-      <c r="G7" s="48">
-        <v>94</v>
-      </c>
-      <c r="H7" s="33">
-        <f t="shared" si="0"/>
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="33" t="s">
         <v>124</v>
       </c>
@@ -42746,17 +42706,10 @@
         <v>89</v>
       </c>
       <c r="F8" s="33">
-        <v>29</v>
-      </c>
-      <c r="G8" s="48">
-        <v>30</v>
-      </c>
-      <c r="H8" s="33">
-        <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="33" t="s">
         <v>129</v>
       </c>
@@ -42770,17 +42723,10 @@
         <v>89</v>
       </c>
       <c r="F9" s="33">
-        <v>142</v>
-      </c>
-      <c r="G9" s="48">
-        <v>165</v>
-      </c>
-      <c r="H9" s="33">
-        <f t="shared" si="0"/>
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="33" t="s">
         <v>496</v>
       </c>
@@ -42794,17 +42740,10 @@
         <v>89</v>
       </c>
       <c r="F10" s="33">
-        <v>164</v>
-      </c>
-      <c r="G10" s="48">
-        <v>67</v>
-      </c>
-      <c r="H10" s="33">
-        <f t="shared" si="0"/>
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="33" t="s">
         <v>189</v>
       </c>
@@ -42818,17 +42757,10 @@
         <v>89</v>
       </c>
       <c r="F11" s="33">
-        <v>5537</v>
-      </c>
-      <c r="G11" s="48">
-        <v>4138</v>
-      </c>
-      <c r="H11" s="33">
-        <f t="shared" si="0"/>
         <v>9675</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="33" t="s">
         <v>511</v>
       </c>
@@ -42841,13 +42773,11 @@
       <c r="E12" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="H12" s="33">
-        <f t="shared" si="0"/>
+      <c r="F12" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="33" t="s">
         <v>512</v>
       </c>
@@ -42860,13 +42790,11 @@
       <c r="E13" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="H13" s="33">
-        <f t="shared" si="0"/>
+      <c r="F13" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="33" t="s">
         <v>513</v>
       </c>
@@ -42882,12 +42810,8 @@
       <c r="F14" s="33">
         <v>1</v>
       </c>
-      <c r="H14" s="33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="33" t="s">
         <v>898</v>
       </c>
@@ -42901,17 +42825,10 @@
         <v>89</v>
       </c>
       <c r="F15" s="33">
-        <v>33</v>
-      </c>
-      <c r="G15" s="48">
-        <v>66</v>
-      </c>
-      <c r="H15" s="33">
-        <f t="shared" si="0"/>
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="33" t="s">
         <v>131</v>
       </c>
@@ -42924,13 +42841,11 @@
       <c r="E16" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="H16" s="33">
-        <f t="shared" si="0"/>
+      <c r="F16" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="33" t="s">
         <v>142</v>
       </c>
@@ -42943,13 +42858,11 @@
       <c r="E17" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="H17" s="33">
-        <f t="shared" si="0"/>
+      <c r="F17" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="33" t="s">
         <v>133</v>
       </c>
@@ -42963,17 +42876,10 @@
         <v>89</v>
       </c>
       <c r="F18" s="33">
-        <v>3</v>
-      </c>
-      <c r="G18" s="48">
-        <v>2</v>
-      </c>
-      <c r="H18" s="33">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="33" t="s">
         <v>126</v>
       </c>
@@ -42987,17 +42893,10 @@
         <v>89</v>
       </c>
       <c r="F19" s="33">
-        <v>39</v>
-      </c>
-      <c r="G19" s="48">
-        <v>19</v>
-      </c>
-      <c r="H19" s="33">
-        <f t="shared" si="0"/>
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="33" t="s">
         <v>515</v>
       </c>
@@ -43011,17 +42910,10 @@
         <v>89</v>
       </c>
       <c r="F20" s="33">
-        <v>10</v>
-      </c>
-      <c r="G20" s="48">
-        <v>12</v>
-      </c>
-      <c r="H20" s="33">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="33" t="s">
         <v>516</v>
       </c>
@@ -43035,17 +42927,10 @@
         <v>89</v>
       </c>
       <c r="F21" s="33">
-        <v>32</v>
-      </c>
-      <c r="G21" s="48">
-        <v>24</v>
-      </c>
-      <c r="H21" s="33">
-        <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="33" t="s">
         <v>497</v>
       </c>
@@ -43059,17 +42944,10 @@
         <v>89</v>
       </c>
       <c r="F22" s="33">
-        <v>1</v>
-      </c>
-      <c r="G22" s="48">
-        <v>1</v>
-      </c>
-      <c r="H22" s="33">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="33" t="s">
         <v>135</v>
       </c>
@@ -43083,17 +42961,10 @@
         <v>89</v>
       </c>
       <c r="F23" s="33">
-        <v>2</v>
-      </c>
-      <c r="G23" s="48">
-        <v>1</v>
-      </c>
-      <c r="H23" s="33">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="33" t="s">
         <v>144</v>
       </c>
@@ -43106,13 +42977,11 @@
       <c r="E24" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="H24" s="33">
-        <f t="shared" si="0"/>
+      <c r="F24" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="33" t="s">
         <v>134</v>
       </c>
@@ -43126,17 +42995,10 @@
         <v>89</v>
       </c>
       <c r="F25" s="33">
-        <v>17</v>
-      </c>
-      <c r="G25" s="48">
-        <v>27</v>
-      </c>
-      <c r="H25" s="33">
-        <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="33" t="s">
         <v>517</v>
       </c>
@@ -43150,17 +43012,10 @@
         <v>89</v>
       </c>
       <c r="F26" s="33">
-        <v>1</v>
-      </c>
-      <c r="G26" s="48">
-        <v>2</v>
-      </c>
-      <c r="H26" s="33">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="33" t="s">
         <v>164</v>
       </c>
@@ -43174,17 +43029,10 @@
         <v>84</v>
       </c>
       <c r="F27" s="33">
-        <v>16</v>
-      </c>
-      <c r="G27" s="48">
-        <v>6</v>
-      </c>
-      <c r="H27" s="33">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="33" t="s">
         <v>518</v>
       </c>
@@ -43198,17 +43046,10 @@
         <v>84</v>
       </c>
       <c r="F28" s="33">
-        <v>4</v>
-      </c>
-      <c r="G28" s="48">
-        <v>1</v>
-      </c>
-      <c r="H28" s="33">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="33" t="s">
         <v>502</v>
       </c>
@@ -43222,17 +43063,10 @@
         <v>89</v>
       </c>
       <c r="F29" s="33">
-        <v>2978</v>
-      </c>
-      <c r="G29" s="48">
-        <v>2330</v>
-      </c>
-      <c r="H29" s="33">
-        <f t="shared" si="0"/>
         <v>5308</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="33" t="s">
         <v>522</v>
       </c>
@@ -43246,17 +43080,10 @@
         <v>89</v>
       </c>
       <c r="F30" s="33">
-        <v>66</v>
-      </c>
-      <c r="G30" s="48">
-        <v>55</v>
-      </c>
-      <c r="H30" s="33">
-        <f t="shared" si="0"/>
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="33" t="s">
         <v>519</v>
       </c>
@@ -43270,17 +43097,10 @@
         <v>89</v>
       </c>
       <c r="F31" s="33">
-        <v>184</v>
-      </c>
-      <c r="G31" s="48">
-        <v>97</v>
-      </c>
-      <c r="H31" s="33">
-        <f t="shared" si="0"/>
         <v>281</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="33" t="s">
         <v>520</v>
       </c>
@@ -43294,17 +43114,10 @@
         <v>89</v>
       </c>
       <c r="F32" s="33">
-        <v>87</v>
-      </c>
-      <c r="G32" s="48">
-        <v>83</v>
-      </c>
-      <c r="H32" s="33">
-        <f t="shared" si="0"/>
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="33" t="s">
         <v>521</v>
       </c>
@@ -43318,17 +43131,10 @@
         <v>89</v>
       </c>
       <c r="F33" s="33">
-        <v>23</v>
-      </c>
-      <c r="G33" s="48">
-        <v>18</v>
-      </c>
-      <c r="H33" s="33">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="33" t="s">
         <v>523</v>
       </c>
@@ -43342,17 +43148,10 @@
         <v>89</v>
       </c>
       <c r="F34" s="33">
-        <v>17</v>
-      </c>
-      <c r="G34" s="48">
-        <v>3</v>
-      </c>
-      <c r="H34" s="33">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="33" t="s">
         <v>524</v>
       </c>
@@ -43366,17 +43165,10 @@
         <v>89</v>
       </c>
       <c r="F35" s="33">
-        <v>57</v>
-      </c>
-      <c r="G35" s="48">
-        <v>26</v>
-      </c>
-      <c r="H35" s="33">
-        <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="33" t="s">
         <v>213</v>
       </c>
@@ -43390,17 +43182,10 @@
         <v>89</v>
       </c>
       <c r="F36" s="33">
-        <v>11</v>
-      </c>
-      <c r="G36" s="48">
-        <v>11</v>
-      </c>
-      <c r="H36" s="33">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="33" t="s">
         <v>525</v>
       </c>
@@ -43414,17 +43199,10 @@
         <v>89</v>
       </c>
       <c r="F37" s="33">
-        <v>5</v>
-      </c>
-      <c r="G37" s="48">
-        <v>1</v>
-      </c>
-      <c r="H37" s="33">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="33" t="s">
         <v>498</v>
       </c>
@@ -43438,17 +43216,10 @@
         <v>89</v>
       </c>
       <c r="F38" s="33">
-        <v>244</v>
-      </c>
-      <c r="G38" s="48">
-        <v>104</v>
-      </c>
-      <c r="H38" s="33">
-        <f t="shared" si="0"/>
         <v>348</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="33" t="s">
         <v>526</v>
       </c>
@@ -43462,17 +43233,10 @@
         <v>89</v>
       </c>
       <c r="F39" s="33">
-        <v>14</v>
-      </c>
-      <c r="G39" s="48">
-        <v>5</v>
-      </c>
-      <c r="H39" s="33">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="33" t="s">
         <v>899</v>
       </c>
@@ -43486,17 +43250,10 @@
         <v>24</v>
       </c>
       <c r="F40" s="33">
-        <v>74</v>
-      </c>
-      <c r="G40" s="48">
-        <v>39</v>
-      </c>
-      <c r="H40" s="33">
-        <f t="shared" si="0"/>
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="33" t="s">
         <v>900</v>
       </c>
@@ -43510,17 +43267,10 @@
         <v>24</v>
       </c>
       <c r="F41" s="33">
-        <v>799</v>
-      </c>
-      <c r="G41" s="48">
-        <v>453</v>
-      </c>
-      <c r="H41" s="33">
-        <f t="shared" si="0"/>
         <v>1252</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B42" s="33" t="s">
         <v>901</v>
       </c>
@@ -43534,17 +43284,10 @@
         <v>24</v>
       </c>
       <c r="F42" s="33">
-        <v>344</v>
-      </c>
-      <c r="G42" s="48">
-        <v>130</v>
-      </c>
-      <c r="H42" s="33">
-        <f t="shared" si="0"/>
         <v>474</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="33" t="s">
         <v>902</v>
       </c>
@@ -43558,17 +43301,10 @@
         <v>24</v>
       </c>
       <c r="F43" s="33">
-        <v>339</v>
-      </c>
-      <c r="G43" s="48">
-        <v>114</v>
-      </c>
-      <c r="H43" s="33">
-        <f t="shared" si="0"/>
         <v>453</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="33" t="s">
         <v>903</v>
       </c>
@@ -43582,17 +43318,10 @@
         <v>24</v>
       </c>
       <c r="F44" s="33">
-        <v>212</v>
-      </c>
-      <c r="G44" s="48">
-        <v>77</v>
-      </c>
-      <c r="H44" s="33">
-        <f t="shared" si="0"/>
         <v>289</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="33" t="s">
         <v>904</v>
       </c>
@@ -43606,17 +43335,10 @@
         <v>24</v>
       </c>
       <c r="F45" s="33">
-        <v>47</v>
-      </c>
-      <c r="G45" s="48">
-        <v>29</v>
-      </c>
-      <c r="H45" s="33">
-        <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B46" s="33" t="s">
         <v>905</v>
       </c>
@@ -43630,17 +43352,10 @@
         <v>24</v>
       </c>
       <c r="F46" s="33">
-        <v>453</v>
-      </c>
-      <c r="G46" s="48">
-        <v>195</v>
-      </c>
-      <c r="H46" s="33">
-        <f t="shared" si="0"/>
         <v>648</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="33" t="s">
         <v>534</v>
       </c>
@@ -43654,17 +43369,10 @@
         <v>24</v>
       </c>
       <c r="F47" s="33">
-        <v>5</v>
-      </c>
-      <c r="G47" s="48">
-        <v>4</v>
-      </c>
-      <c r="H47" s="33">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="33" t="s">
         <v>1285</v>
       </c>
@@ -43678,17 +43386,10 @@
         <v>84</v>
       </c>
       <c r="F48" s="33">
-        <v>53</v>
-      </c>
-      <c r="G48" s="48">
-        <v>28</v>
-      </c>
-      <c r="H48" s="33">
-        <f t="shared" si="0"/>
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="33" t="s">
         <v>536</v>
       </c>
@@ -43702,17 +43403,10 @@
         <v>14</v>
       </c>
       <c r="F49" s="33">
-        <v>17</v>
-      </c>
-      <c r="G49" s="48">
-        <v>22</v>
-      </c>
-      <c r="H49" s="33">
-        <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="33" t="s">
         <v>537</v>
       </c>
@@ -43726,17 +43420,10 @@
         <v>84</v>
       </c>
       <c r="F50" s="33">
-        <v>1</v>
-      </c>
-      <c r="G50" s="48">
-        <v>1</v>
-      </c>
-      <c r="H50" s="33">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="33" t="s">
         <v>21</v>
       </c>
@@ -43750,17 +43437,10 @@
         <v>14</v>
       </c>
       <c r="F51" s="33">
-        <v>339</v>
-      </c>
-      <c r="G51" s="48">
-        <v>196</v>
-      </c>
-      <c r="H51" s="33">
-        <f t="shared" si="0"/>
         <v>535</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="s">
         <v>538</v>
       </c>
@@ -43774,17 +43454,10 @@
         <v>14</v>
       </c>
       <c r="F52" s="33">
-        <v>31</v>
-      </c>
-      <c r="G52" s="48">
-        <v>12</v>
-      </c>
-      <c r="H52" s="33">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="33" t="s">
         <v>72</v>
       </c>
@@ -43798,17 +43471,10 @@
         <v>14</v>
       </c>
       <c r="F53" s="33">
-        <v>8</v>
-      </c>
-      <c r="G53" s="48">
-        <v>9</v>
-      </c>
-      <c r="H53" s="33">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="33" t="s">
         <v>539</v>
       </c>
@@ -43822,17 +43488,10 @@
         <v>24</v>
       </c>
       <c r="F54" s="33">
-        <v>54</v>
-      </c>
-      <c r="G54" s="48">
-        <v>18</v>
-      </c>
-      <c r="H54" s="33">
-        <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="33" t="s">
         <v>540</v>
       </c>
@@ -43846,17 +43505,10 @@
         <v>14</v>
       </c>
       <c r="F55" s="33">
-        <v>142</v>
-      </c>
-      <c r="G55" s="48">
-        <v>61</v>
-      </c>
-      <c r="H55" s="33">
-        <f t="shared" si="0"/>
         <v>203</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" s="33" t="s">
         <v>541</v>
       </c>
@@ -43870,17 +43522,10 @@
         <v>84</v>
       </c>
       <c r="F56" s="33">
-        <v>21</v>
-      </c>
-      <c r="G56" s="48">
-        <v>6</v>
-      </c>
-      <c r="H56" s="33">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" s="33" t="s">
         <v>542</v>
       </c>
@@ -43894,17 +43539,10 @@
         <v>14</v>
       </c>
       <c r="F57" s="33">
-        <v>64</v>
-      </c>
-      <c r="G57" s="48">
-        <v>75</v>
-      </c>
-      <c r="H57" s="33">
-        <f t="shared" si="0"/>
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="33" t="s">
         <v>543</v>
       </c>
@@ -43917,16 +43555,11 @@
       <c r="E58" s="153" t="s">
         <v>86</v>
       </c>
-      <c r="F58" s="33"/>
-      <c r="G58" s="48">
+      <c r="F58" s="33">
         <v>2</v>
       </c>
-      <c r="H58" s="33">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="33" t="s">
         <v>544</v>
       </c>
@@ -43940,17 +43573,10 @@
         <v>86</v>
       </c>
       <c r="F59" s="33">
-        <v>1</v>
-      </c>
-      <c r="G59" s="48">
-        <v>2</v>
-      </c>
-      <c r="H59" s="33">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="53"/>
       <c r="B60" s="35" t="s">
         <v>545</v>
@@ -43964,18 +43590,11 @@
       <c r="E60" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="F60" s="35">
-        <v>8</v>
-      </c>
-      <c r="G60" s="53">
-        <v>2</v>
-      </c>
-      <c r="H60" s="33">
-        <f t="shared" si="0"/>
+      <c r="F60" s="33">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="48" t="s">
         <v>508</v>
       </c>
@@ -43992,17 +43611,10 @@
         <v>84</v>
       </c>
       <c r="F61" s="50">
-        <v>16</v>
-      </c>
-      <c r="G61" s="48">
-        <v>7</v>
-      </c>
-      <c r="H61" s="50">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="33" t="s">
         <v>546</v>
       </c>
@@ -44016,17 +43628,10 @@
         <v>89</v>
       </c>
       <c r="F62" s="33">
-        <v>59</v>
-      </c>
-      <c r="G62" s="48">
-        <v>46</v>
-      </c>
-      <c r="H62" s="33">
-        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="33" t="s">
         <v>547</v>
       </c>
@@ -44040,17 +43645,10 @@
         <v>89</v>
       </c>
       <c r="F63" s="33">
-        <v>32</v>
-      </c>
-      <c r="G63" s="48">
-        <v>30</v>
-      </c>
-      <c r="H63" s="33">
-        <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B64" s="33" t="s">
         <v>548</v>
       </c>
@@ -44064,17 +43662,10 @@
         <v>89</v>
       </c>
       <c r="F64" s="33">
-        <v>61</v>
-      </c>
-      <c r="G64" s="48">
-        <v>24</v>
-      </c>
-      <c r="H64" s="33">
-        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B65" s="33" t="s">
         <v>63</v>
       </c>
@@ -44088,17 +43679,10 @@
         <v>89</v>
       </c>
       <c r="F65" s="33">
-        <v>65</v>
-      </c>
-      <c r="G65" s="48">
-        <v>36</v>
-      </c>
-      <c r="H65" s="33">
-        <f t="shared" si="0"/>
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="33" t="s">
         <v>499</v>
       </c>
@@ -44112,17 +43696,10 @@
         <v>89</v>
       </c>
       <c r="F66" s="33">
-        <v>9</v>
-      </c>
-      <c r="G66" s="48">
-        <v>11</v>
-      </c>
-      <c r="H66" s="33">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="33" t="s">
         <v>549</v>
       </c>
@@ -44136,17 +43713,10 @@
         <v>84</v>
       </c>
       <c r="F67" s="33">
-        <v>120</v>
-      </c>
-      <c r="G67" s="48">
-        <v>65</v>
-      </c>
-      <c r="H67" s="33">
-        <f t="shared" ref="H67:H130" si="1">F67+G67</f>
         <v>185</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="33" t="s">
         <v>550</v>
       </c>
@@ -44160,17 +43730,10 @@
         <v>68</v>
       </c>
       <c r="F68" s="33">
-        <v>1673</v>
-      </c>
-      <c r="G68" s="48">
-        <v>1098</v>
-      </c>
-      <c r="H68" s="33">
-        <f t="shared" si="1"/>
         <v>2771</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="33" t="s">
         <v>551</v>
       </c>
@@ -44184,17 +43747,10 @@
         <v>14</v>
       </c>
       <c r="F69" s="33">
-        <v>20</v>
-      </c>
-      <c r="G69" s="48">
-        <v>26</v>
-      </c>
-      <c r="H69" s="33">
-        <f t="shared" si="1"/>
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="33" t="s">
         <v>552</v>
       </c>
@@ -44208,17 +43764,10 @@
         <v>14</v>
       </c>
       <c r="F70" s="33">
-        <v>80</v>
-      </c>
-      <c r="G70" s="48">
-        <v>101</v>
-      </c>
-      <c r="H70" s="33">
-        <f t="shared" si="1"/>
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="33" t="s">
         <v>553</v>
       </c>
@@ -44232,17 +43781,10 @@
         <v>14</v>
       </c>
       <c r="F71" s="33">
-        <v>105</v>
-      </c>
-      <c r="G71" s="48">
-        <v>275</v>
-      </c>
-      <c r="H71" s="33">
-        <f t="shared" si="1"/>
         <v>380</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="33" t="s">
         <v>554</v>
       </c>
@@ -44256,17 +43798,10 @@
         <v>14</v>
       </c>
       <c r="F72" s="33">
-        <v>27</v>
-      </c>
-      <c r="G72" s="48">
-        <v>51</v>
-      </c>
-      <c r="H72" s="33">
-        <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B73" s="33" t="s">
         <v>34</v>
       </c>
@@ -44280,17 +43815,10 @@
         <v>14</v>
       </c>
       <c r="F73" s="33">
-        <v>49</v>
-      </c>
-      <c r="G73" s="48">
-        <v>69</v>
-      </c>
-      <c r="H73" s="33">
-        <f t="shared" si="1"/>
         <v>118</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B74" s="33" t="s">
         <v>555</v>
       </c>
@@ -44303,16 +43831,11 @@
       <c r="E74" s="153" t="s">
         <v>14</v>
       </c>
-      <c r="F74" s="33"/>
-      <c r="G74" s="48">
+      <c r="F74" s="33">
         <v>1</v>
       </c>
-      <c r="H74" s="33">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="33" t="s">
         <v>556</v>
       </c>
@@ -44326,17 +43849,10 @@
         <v>84</v>
       </c>
       <c r="F75" s="33">
-        <v>18</v>
-      </c>
-      <c r="G75" s="48">
-        <v>22</v>
-      </c>
-      <c r="H75" s="33">
-        <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="37"/>
       <c r="B76" s="33" t="s">
         <v>33</v>
@@ -44351,17 +43867,10 @@
         <v>14</v>
       </c>
       <c r="F76" s="33">
-        <v>1</v>
-      </c>
-      <c r="G76" s="37">
-        <v>6</v>
-      </c>
-      <c r="H76" s="33">
-        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="37"/>
       <c r="B77" s="33" t="s">
         <v>557</v>
@@ -44376,17 +43885,10 @@
         <v>14</v>
       </c>
       <c r="F77" s="33">
-        <v>2</v>
-      </c>
-      <c r="G77" s="37">
-        <v>3</v>
-      </c>
-      <c r="H77" s="33">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="37"/>
       <c r="B78" s="33" t="s">
         <v>558</v>
@@ -44401,17 +43903,10 @@
         <v>84</v>
       </c>
       <c r="F78" s="33">
-        <v>77</v>
-      </c>
-      <c r="G78" s="37">
-        <v>43</v>
-      </c>
-      <c r="H78" s="33">
-        <f t="shared" si="1"/>
         <v>120</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="37"/>
       <c r="B79" s="33" t="s">
         <v>559</v>
@@ -44426,17 +43921,10 @@
         <v>84</v>
       </c>
       <c r="F79" s="33">
-        <v>2</v>
-      </c>
-      <c r="G79" s="37">
-        <v>3</v>
-      </c>
-      <c r="H79" s="33">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="53"/>
       <c r="B80" s="35" t="s">
         <v>560</v>
@@ -44450,18 +43938,11 @@
       <c r="E80" s="159" t="s">
         <v>84</v>
       </c>
-      <c r="F80" s="35">
-        <v>38</v>
-      </c>
-      <c r="G80" s="53">
-        <v>11</v>
-      </c>
-      <c r="H80" s="33">
-        <f t="shared" si="1"/>
+      <c r="F80" s="33">
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="48" t="s">
         <v>106</v>
       </c>
@@ -44477,18 +43958,11 @@
       <c r="E81" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="F81" s="33">
-        <v>20</v>
-      </c>
-      <c r="G81" s="48">
-        <v>21</v>
-      </c>
-      <c r="H81" s="50">
-        <f t="shared" si="1"/>
+      <c r="F81" s="50">
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B82" s="33" t="s">
         <v>562</v>
       </c>
@@ -44502,17 +43976,10 @@
         <v>68</v>
       </c>
       <c r="F82" s="33">
-        <v>182</v>
-      </c>
-      <c r="G82" s="48">
-        <v>81</v>
-      </c>
-      <c r="H82" s="33">
-        <f t="shared" si="1"/>
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B83" s="33" t="s">
         <v>500</v>
       </c>
@@ -44526,17 +43993,10 @@
         <v>68</v>
       </c>
       <c r="F83" s="33">
-        <v>3716</v>
-      </c>
-      <c r="G83" s="48">
-        <v>2434</v>
-      </c>
-      <c r="H83" s="33">
-        <f t="shared" si="1"/>
         <v>6150</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="37"/>
       <c r="B84" s="33" t="s">
         <v>563</v>
@@ -44551,17 +44011,10 @@
         <v>68</v>
       </c>
       <c r="F84" s="33">
-        <v>177</v>
-      </c>
-      <c r="G84" s="37">
-        <v>126</v>
-      </c>
-      <c r="H84" s="33">
-        <f t="shared" si="1"/>
         <v>303</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="37"/>
       <c r="B85" s="33" t="s">
         <v>1234</v>
@@ -44576,17 +44029,10 @@
         <v>68</v>
       </c>
       <c r="F85" s="33">
-        <v>476</v>
-      </c>
-      <c r="G85" s="37">
-        <v>420</v>
-      </c>
-      <c r="H85" s="33">
-        <f t="shared" si="1"/>
         <v>896</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="37"/>
       <c r="B86" s="33" t="s">
         <v>565</v>
@@ -44601,17 +44047,10 @@
         <v>68</v>
       </c>
       <c r="F86" s="33">
-        <v>93</v>
-      </c>
-      <c r="G86" s="37">
-        <v>74</v>
-      </c>
-      <c r="H86" s="33">
-        <f t="shared" si="1"/>
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="37"/>
       <c r="B87" s="33" t="s">
         <v>566</v>
@@ -44626,17 +44065,10 @@
         <v>68</v>
       </c>
       <c r="F87" s="33">
-        <v>12</v>
-      </c>
-      <c r="G87" s="37">
-        <v>9</v>
-      </c>
-      <c r="H87" s="33">
-        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="37"/>
       <c r="B88" s="33" t="s">
         <v>675</v>
@@ -44651,17 +44083,10 @@
         <v>68</v>
       </c>
       <c r="F88" s="33">
-        <v>15</v>
-      </c>
-      <c r="G88" s="37">
-        <v>4</v>
-      </c>
-      <c r="H88" s="33">
-        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="53"/>
       <c r="B89" s="35" t="s">
         <v>567</v>
@@ -44675,18 +44100,11 @@
       <c r="E89" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="F89" s="35">
-        <v>5</v>
-      </c>
-      <c r="G89" s="53">
-        <v>4</v>
-      </c>
-      <c r="H89" s="33">
-        <f t="shared" si="1"/>
+      <c r="F89" s="33">
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="48" t="s">
         <v>107</v>
       </c>
@@ -44702,18 +44120,11 @@
       <c r="E90" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="F90" s="33">
-        <v>1</v>
-      </c>
-      <c r="G90" s="48">
-        <v>1</v>
-      </c>
-      <c r="H90" s="50">
-        <f t="shared" si="1"/>
+      <c r="F90" s="50">
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B91" s="33" t="s">
         <v>569</v>
       </c>
@@ -44727,17 +44138,10 @@
         <v>84</v>
       </c>
       <c r="F91" s="33">
-        <v>11</v>
-      </c>
-      <c r="G91" s="48">
-        <v>11</v>
-      </c>
-      <c r="H91" s="33">
-        <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="33" t="s">
         <v>570</v>
       </c>
@@ -44751,17 +44155,10 @@
         <v>84</v>
       </c>
       <c r="F92" s="33">
-        <v>14</v>
-      </c>
-      <c r="G92" s="48">
-        <v>4</v>
-      </c>
-      <c r="H92" s="33">
-        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B93" s="33" t="s">
         <v>190</v>
       </c>
@@ -44775,17 +44172,10 @@
         <v>84</v>
       </c>
       <c r="F93" s="33">
-        <v>99</v>
-      </c>
-      <c r="G93" s="48">
-        <v>63</v>
-      </c>
-      <c r="H93" s="33">
-        <f t="shared" si="1"/>
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B94" s="33" t="s">
         <v>571</v>
       </c>
@@ -44799,17 +44189,10 @@
         <v>14</v>
       </c>
       <c r="F94" s="33">
-        <v>103</v>
-      </c>
-      <c r="G94" s="48">
-        <v>65</v>
-      </c>
-      <c r="H94" s="33">
-        <f t="shared" si="1"/>
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B95" s="33" t="s">
         <v>301</v>
       </c>
@@ -44823,17 +44206,10 @@
         <v>84</v>
       </c>
       <c r="F95" s="33">
-        <v>1060</v>
-      </c>
-      <c r="G95" s="48">
-        <v>633</v>
-      </c>
-      <c r="H95" s="33">
-        <f t="shared" si="1"/>
         <v>1693</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B96" s="33" t="s">
         <v>300</v>
       </c>
@@ -44847,17 +44223,10 @@
         <v>84</v>
       </c>
       <c r="F96" s="33">
-        <v>3168</v>
-      </c>
-      <c r="G96" s="48">
-        <v>1773</v>
-      </c>
-      <c r="H96" s="33">
-        <f t="shared" si="1"/>
         <v>4941</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B97" s="33" t="s">
         <v>572</v>
       </c>
@@ -44871,17 +44240,10 @@
         <v>84</v>
       </c>
       <c r="F97" s="33">
-        <v>172</v>
-      </c>
-      <c r="G97" s="48">
-        <v>292</v>
-      </c>
-      <c r="H97" s="33">
-        <f t="shared" si="1"/>
         <v>464</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B98" s="33" t="s">
         <v>194</v>
       </c>
@@ -44895,17 +44257,10 @@
         <v>84</v>
       </c>
       <c r="F98" s="33">
-        <v>80</v>
-      </c>
-      <c r="G98" s="48">
-        <v>33</v>
-      </c>
-      <c r="H98" s="33">
-        <f t="shared" si="1"/>
         <v>113</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B99" s="33" t="s">
         <v>573</v>
       </c>
@@ -44919,17 +44274,10 @@
         <v>84</v>
       </c>
       <c r="F99" s="33">
-        <v>37</v>
-      </c>
-      <c r="G99" s="48">
-        <v>35</v>
-      </c>
-      <c r="H99" s="33">
-        <f t="shared" si="1"/>
         <v>72</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B100" s="33" t="s">
         <v>574</v>
       </c>
@@ -44943,17 +44291,10 @@
         <v>84</v>
       </c>
       <c r="F100" s="33">
-        <v>13</v>
-      </c>
-      <c r="G100" s="48">
-        <v>8</v>
-      </c>
-      <c r="H100" s="33">
-        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="37"/>
       <c r="B101" s="33" t="s">
         <v>69</v>
@@ -44968,17 +44309,10 @@
         <v>14</v>
       </c>
       <c r="F101" s="33">
-        <v>41</v>
-      </c>
-      <c r="G101" s="37">
-        <v>41</v>
-      </c>
-      <c r="H101" s="33">
-        <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="37"/>
       <c r="B102" s="33" t="s">
         <v>575</v>
@@ -44993,17 +44327,10 @@
         <v>14</v>
       </c>
       <c r="F102" s="33">
-        <v>3</v>
-      </c>
-      <c r="G102" s="37">
-        <v>3</v>
-      </c>
-      <c r="H102" s="33">
-        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="53"/>
       <c r="B103" s="35" t="s">
         <v>576</v>
@@ -45017,18 +44344,11 @@
       <c r="E103" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="F103" s="35">
-        <v>11</v>
-      </c>
-      <c r="G103" s="53">
-        <v>23</v>
-      </c>
-      <c r="H103" s="33">
-        <f t="shared" si="1"/>
+      <c r="F103" s="33">
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>108</v>
       </c>
@@ -45044,18 +44364,11 @@
       <c r="E104" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F104" s="33">
-        <v>20</v>
-      </c>
-      <c r="G104" s="48">
-        <v>12</v>
-      </c>
-      <c r="H104" s="50">
-        <f t="shared" si="1"/>
+      <c r="F104" s="50">
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B105" s="33" t="s">
         <v>577</v>
       </c>
@@ -45069,17 +44382,10 @@
         <v>84</v>
       </c>
       <c r="F105" s="33">
-        <v>62</v>
-      </c>
-      <c r="G105" s="48">
-        <v>31</v>
-      </c>
-      <c r="H105" s="33">
-        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B106" s="33" t="s">
         <v>578</v>
       </c>
@@ -45095,12 +44401,8 @@
       <c r="F106" s="33">
         <v>2</v>
       </c>
-      <c r="H106" s="33">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B107" s="33" t="s">
         <v>579</v>
       </c>
@@ -45114,17 +44416,10 @@
         <v>84</v>
       </c>
       <c r="F107" s="33">
-        <v>146</v>
-      </c>
-      <c r="G107" s="48">
-        <v>63</v>
-      </c>
-      <c r="H107" s="33">
-        <f t="shared" si="1"/>
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B108" s="33" t="s">
         <v>907</v>
       </c>
@@ -45138,17 +44433,10 @@
         <v>84</v>
       </c>
       <c r="F108" s="33">
-        <v>132</v>
-      </c>
-      <c r="G108" s="48">
-        <v>128</v>
-      </c>
-      <c r="H108" s="33">
-        <f t="shared" si="1"/>
         <v>260</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B109" s="33" t="s">
         <v>501</v>
       </c>
@@ -45162,17 +44450,10 @@
         <v>89</v>
       </c>
       <c r="F109" s="33">
-        <v>486</v>
-      </c>
-      <c r="G109" s="48">
-        <v>577</v>
-      </c>
-      <c r="H109" s="33">
-        <f t="shared" si="1"/>
         <v>1063</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B110" s="33" t="s">
         <v>581</v>
       </c>
@@ -45186,17 +44467,10 @@
         <v>89</v>
       </c>
       <c r="F110" s="33">
-        <v>190</v>
-      </c>
-      <c r="G110" s="48">
-        <v>178</v>
-      </c>
-      <c r="H110" s="33">
-        <f t="shared" si="1"/>
         <v>368</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B111" s="33" t="s">
         <v>150</v>
       </c>
@@ -45209,13 +44483,11 @@
       <c r="E111" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F111" s="33"/>
-      <c r="H111" s="33">
-        <f t="shared" si="1"/>
+      <c r="F111" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="33" t="s">
         <v>582</v>
       </c>
@@ -45231,12 +44503,8 @@
       <c r="F112" s="33">
         <v>4</v>
       </c>
-      <c r="H112" s="33">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B113" s="33" t="s">
         <v>504</v>
       </c>
@@ -45250,17 +44518,10 @@
         <v>84</v>
       </c>
       <c r="F113" s="33">
-        <v>287</v>
-      </c>
-      <c r="G113" s="48">
-        <v>110</v>
-      </c>
-      <c r="H113" s="33">
-        <f t="shared" si="1"/>
         <v>397</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B114" s="33" t="s">
         <v>583</v>
       </c>
@@ -45274,17 +44535,10 @@
         <v>84</v>
       </c>
       <c r="F114" s="33">
-        <v>91</v>
-      </c>
-      <c r="G114" s="48">
-        <v>39</v>
-      </c>
-      <c r="H114" s="33">
-        <f t="shared" si="1"/>
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B115" s="33" t="s">
         <v>584</v>
       </c>
@@ -45298,17 +44552,10 @@
         <v>84</v>
       </c>
       <c r="F115" s="33">
-        <v>162</v>
-      </c>
-      <c r="G115" s="48">
-        <v>96</v>
-      </c>
-      <c r="H115" s="33">
-        <f t="shared" si="1"/>
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B116" s="33" t="s">
         <v>585</v>
       </c>
@@ -45322,17 +44569,10 @@
         <v>84</v>
       </c>
       <c r="F116" s="33">
-        <v>52</v>
-      </c>
-      <c r="G116" s="48">
-        <v>36</v>
-      </c>
-      <c r="H116" s="33">
-        <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="33" t="s">
         <v>586</v>
       </c>
@@ -45346,17 +44586,10 @@
         <v>84</v>
       </c>
       <c r="F117" s="33">
-        <v>11</v>
-      </c>
-      <c r="G117" s="48">
-        <v>3</v>
-      </c>
-      <c r="H117" s="33">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B118" s="33" t="s">
         <v>587</v>
       </c>
@@ -45372,12 +44605,8 @@
       <c r="F118" s="33">
         <v>3</v>
       </c>
-      <c r="H118" s="33">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="37"/>
       <c r="B119" s="33" t="s">
         <v>505</v>
@@ -45392,17 +44621,10 @@
         <v>14</v>
       </c>
       <c r="F119" s="33">
-        <v>313</v>
-      </c>
-      <c r="G119" s="37">
-        <v>148</v>
-      </c>
-      <c r="H119" s="33">
-        <f t="shared" si="1"/>
         <v>461</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="37"/>
       <c r="B120" s="33" t="s">
         <v>588</v>
@@ -45417,17 +44639,10 @@
         <v>14</v>
       </c>
       <c r="F120" s="33">
-        <v>56</v>
-      </c>
-      <c r="G120" s="37">
-        <v>19</v>
-      </c>
-      <c r="H120" s="33">
-        <f t="shared" si="1"/>
         <v>75</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="37"/>
       <c r="B121" s="33" t="s">
         <v>589</v>
@@ -45442,17 +44657,10 @@
         <v>84</v>
       </c>
       <c r="F121" s="33">
-        <v>95</v>
-      </c>
-      <c r="G121" s="37">
-        <v>48</v>
-      </c>
-      <c r="H121" s="33">
-        <f t="shared" si="1"/>
         <v>143</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="37"/>
       <c r="B122" s="33" t="s">
         <v>590</v>
@@ -45467,17 +44675,10 @@
         <v>84</v>
       </c>
       <c r="F122" s="33">
-        <v>5</v>
-      </c>
-      <c r="G122" s="37">
-        <v>2</v>
-      </c>
-      <c r="H122" s="33">
-        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="37"/>
       <c r="B123" s="33" t="s">
         <v>591</v>
@@ -45492,17 +44693,10 @@
         <v>89</v>
       </c>
       <c r="F123" s="33">
-        <v>33</v>
-      </c>
-      <c r="G123" s="37">
-        <v>22</v>
-      </c>
-      <c r="H123" s="33">
-        <f t="shared" si="1"/>
         <v>55</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="53"/>
       <c r="B124" s="35" t="s">
         <v>908</v>
@@ -45516,18 +44710,11 @@
       <c r="E124" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F124" s="35">
-        <v>28</v>
-      </c>
-      <c r="G124" s="53">
-        <v>6</v>
-      </c>
-      <c r="H124" s="33">
-        <f t="shared" si="1"/>
+      <c r="F124" s="33">
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="48" t="s">
         <v>896</v>
       </c>
@@ -45543,18 +44730,11 @@
       <c r="E125" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="F125" s="33">
-        <v>140</v>
-      </c>
-      <c r="G125" s="48">
-        <v>78</v>
-      </c>
-      <c r="H125" s="50">
-        <f t="shared" si="1"/>
+      <c r="F125" s="50">
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B126" s="33" t="s">
         <v>592</v>
       </c>
@@ -45568,17 +44748,10 @@
         <v>14</v>
       </c>
       <c r="F126" s="33">
-        <v>1837</v>
-      </c>
-      <c r="G126" s="48">
-        <v>1047</v>
-      </c>
-      <c r="H126" s="33">
-        <f t="shared" si="1"/>
         <v>2884</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B127" s="33" t="s">
         <v>593</v>
       </c>
@@ -45591,13 +44764,11 @@
       <c r="E127" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="F127" s="33"/>
-      <c r="H127" s="33">
-        <f t="shared" si="1"/>
+      <c r="F127" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B128" s="33" t="s">
         <v>594</v>
       </c>
@@ -45611,17 +44782,10 @@
         <v>84</v>
       </c>
       <c r="F128" s="33">
-        <v>56</v>
-      </c>
-      <c r="G128" s="48">
-        <v>24</v>
-      </c>
-      <c r="H128" s="33">
-        <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B129" s="33" t="s">
         <v>1286</v>
       </c>
@@ -45635,17 +44799,10 @@
         <v>84</v>
       </c>
       <c r="F129" s="33">
-        <v>19</v>
-      </c>
-      <c r="G129" s="48">
-        <v>7</v>
-      </c>
-      <c r="H129" s="33">
-        <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B130" s="33" t="s">
         <v>596</v>
       </c>
@@ -45659,17 +44816,10 @@
         <v>84</v>
       </c>
       <c r="F130" s="33">
-        <v>25</v>
-      </c>
-      <c r="G130" s="48">
-        <v>35</v>
-      </c>
-      <c r="H130" s="33">
-        <f t="shared" si="1"/>
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B131" s="33" t="s">
         <v>910</v>
       </c>
@@ -45683,17 +44833,10 @@
         <v>84</v>
       </c>
       <c r="F131" s="33">
-        <v>7</v>
-      </c>
-      <c r="G131" s="48">
-        <v>1</v>
-      </c>
-      <c r="H131" s="33">
-        <f t="shared" ref="H131:H194" si="2">F131+G131</f>
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B132" s="33" t="s">
         <v>598</v>
       </c>
@@ -45707,17 +44850,10 @@
         <v>84</v>
       </c>
       <c r="F132" s="33">
-        <v>121</v>
-      </c>
-      <c r="G132" s="48">
-        <v>61</v>
-      </c>
-      <c r="H132" s="33">
-        <f t="shared" si="2"/>
         <v>182</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B133" s="33" t="s">
         <v>599</v>
       </c>
@@ -45733,12 +44869,8 @@
       <c r="F133" s="33">
         <v>4</v>
       </c>
-      <c r="H133" s="33">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B134" s="33" t="s">
         <v>600</v>
       </c>
@@ -45752,17 +44884,10 @@
         <v>84</v>
       </c>
       <c r="F134" s="33">
-        <v>3</v>
-      </c>
-      <c r="G134" s="48">
-        <v>2</v>
-      </c>
-      <c r="H134" s="33">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="37"/>
       <c r="B135" s="33" t="s">
         <v>601</v>
@@ -45777,17 +44902,10 @@
         <v>24</v>
       </c>
       <c r="F135" s="33">
-        <v>41</v>
-      </c>
-      <c r="G135" s="37">
-        <v>16</v>
-      </c>
-      <c r="H135" s="33">
-        <f t="shared" si="2"/>
         <v>57</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="37"/>
       <c r="B136" s="33" t="s">
         <v>602</v>
@@ -45802,17 +44920,10 @@
         <v>84</v>
       </c>
       <c r="F136" s="33">
-        <v>22</v>
-      </c>
-      <c r="G136" s="37">
-        <v>9</v>
-      </c>
-      <c r="H136" s="33">
-        <f t="shared" si="2"/>
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="37"/>
       <c r="B137" s="33" t="s">
         <v>603</v>
@@ -45827,17 +44938,10 @@
         <v>84</v>
       </c>
       <c r="F137" s="33">
-        <v>15</v>
-      </c>
-      <c r="G137" s="37">
-        <v>9</v>
-      </c>
-      <c r="H137" s="33">
-        <f t="shared" si="2"/>
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="37"/>
       <c r="B138" s="33" t="s">
         <v>604</v>
@@ -45852,17 +44956,10 @@
         <v>84</v>
       </c>
       <c r="F138" s="33">
-        <v>48</v>
-      </c>
-      <c r="G138" s="37">
-        <v>14</v>
-      </c>
-      <c r="H138" s="33">
-        <f t="shared" si="2"/>
         <v>62</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="37"/>
       <c r="B139" s="33" t="s">
         <v>605</v>
@@ -45879,13 +44976,8 @@
       <c r="F139" s="33">
         <v>2</v>
       </c>
-      <c r="G139" s="37"/>
-      <c r="H139" s="33">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="168" t="s">
         <v>1287</v>
       </c>
@@ -45902,17 +44994,10 @@
         <v>86</v>
       </c>
       <c r="F140" s="50">
-        <v>72</v>
-      </c>
-      <c r="G140" s="168">
-        <v>47</v>
-      </c>
-      <c r="H140" s="50">
-        <f t="shared" si="2"/>
         <v>119</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="37"/>
       <c r="B141" s="33" t="s">
         <v>608</v>
@@ -45927,17 +45012,10 @@
         <v>84</v>
       </c>
       <c r="F141" s="33">
-        <v>32</v>
-      </c>
-      <c r="G141" s="37">
-        <v>28</v>
-      </c>
-      <c r="H141" s="33">
-        <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="37"/>
       <c r="B142" s="33" t="s">
         <v>609</v>
@@ -45952,17 +45030,10 @@
         <v>84</v>
       </c>
       <c r="F142" s="33">
-        <v>49</v>
-      </c>
-      <c r="G142" s="37">
-        <v>38</v>
-      </c>
-      <c r="H142" s="33">
-        <f t="shared" si="2"/>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="37"/>
       <c r="B143" s="33" t="s">
         <v>506</v>
@@ -45977,17 +45048,10 @@
         <v>89</v>
       </c>
       <c r="F143" s="33">
-        <v>115</v>
-      </c>
-      <c r="G143" s="37">
-        <v>60</v>
-      </c>
-      <c r="H143" s="33">
-        <f t="shared" si="2"/>
         <v>175</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="37"/>
       <c r="B144" s="33" t="s">
         <v>610</v>
@@ -46002,17 +45066,10 @@
         <v>84</v>
       </c>
       <c r="F144" s="33">
-        <v>64</v>
-      </c>
-      <c r="G144" s="37">
-        <v>45</v>
-      </c>
-      <c r="H144" s="33">
-        <f t="shared" si="2"/>
         <v>109</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="37"/>
       <c r="B145" s="33" t="s">
         <v>611</v>
@@ -46027,17 +45084,10 @@
         <v>84</v>
       </c>
       <c r="F145" s="33">
-        <v>10</v>
-      </c>
-      <c r="G145" s="37">
-        <v>6</v>
-      </c>
-      <c r="H145" s="33">
-        <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="37"/>
       <c r="B146" s="33" t="s">
         <v>612</v>
@@ -46052,17 +45102,10 @@
         <v>84</v>
       </c>
       <c r="F146" s="33">
-        <v>1</v>
-      </c>
-      <c r="G146" s="37">
-        <v>1</v>
-      </c>
-      <c r="H146" s="33">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="53"/>
       <c r="B147" s="35" t="s">
         <v>613</v>
@@ -46076,16 +45119,11 @@
       <c r="E147" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F147" s="35">
+      <c r="F147" s="33">
         <v>1</v>
       </c>
-      <c r="G147" s="53"/>
-      <c r="H147" s="33">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="168" t="s">
         <v>897</v>
       </c>
@@ -46102,17 +45140,10 @@
         <v>68</v>
       </c>
       <c r="F148" s="50">
-        <v>29</v>
-      </c>
-      <c r="G148" s="168">
-        <v>26</v>
-      </c>
-      <c r="H148" s="50">
-        <f t="shared" si="2"/>
         <v>55</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="37"/>
       <c r="B149" s="33" t="s">
         <v>616</v>
@@ -46127,17 +45158,10 @@
         <v>89</v>
       </c>
       <c r="F149" s="33">
-        <v>5</v>
-      </c>
-      <c r="G149" s="37">
-        <v>3</v>
-      </c>
-      <c r="H149" s="33">
-        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="37"/>
       <c r="B150" s="33" t="s">
         <v>1276</v>
@@ -46152,17 +45176,10 @@
         <v>89</v>
       </c>
       <c r="F150" s="33">
-        <v>14</v>
-      </c>
-      <c r="G150" s="37">
-        <v>8</v>
-      </c>
-      <c r="H150" s="33">
-        <f t="shared" si="2"/>
         <v>22</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="53"/>
       <c r="B151" s="35" t="s">
         <v>617</v>
@@ -46176,18 +45193,11 @@
       <c r="E151" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F151" s="35">
-        <v>17</v>
-      </c>
-      <c r="G151" s="53">
-        <v>7</v>
-      </c>
-      <c r="H151" s="33">
-        <f t="shared" si="2"/>
+      <c r="F151" s="33">
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="48" t="s">
         <v>618</v>
       </c>
@@ -46203,18 +45213,11 @@
       <c r="E152" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F152" s="33">
-        <v>65</v>
-      </c>
-      <c r="G152" s="48">
-        <v>22</v>
-      </c>
-      <c r="H152" s="50">
-        <f t="shared" si="2"/>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F152" s="50">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B153" s="33" t="s">
         <v>620</v>
       </c>
@@ -46228,17 +45231,10 @@
         <v>84</v>
       </c>
       <c r="F153" s="33">
-        <v>7</v>
-      </c>
-      <c r="G153" s="48">
-        <v>3</v>
-      </c>
-      <c r="H153" s="33">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B154" s="33" t="s">
         <v>621</v>
       </c>
@@ -46251,13 +45247,11 @@
       <c r="E154" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F154" s="33"/>
-      <c r="H154" s="33">
-        <f t="shared" si="2"/>
+      <c r="F154" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B155" s="33" t="s">
         <v>622</v>
       </c>
@@ -46271,17 +45265,10 @@
         <v>84</v>
       </c>
       <c r="F155" s="33">
-        <v>1</v>
-      </c>
-      <c r="G155" s="48">
-        <v>2</v>
-      </c>
-      <c r="H155" s="33">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="168" t="s">
         <v>623</v>
       </c>
@@ -46298,17 +45285,10 @@
         <v>84</v>
       </c>
       <c r="F156" s="50">
-        <v>23</v>
-      </c>
-      <c r="G156" s="168">
-        <v>17</v>
-      </c>
-      <c r="H156" s="50">
-        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B157" s="33" t="s">
         <v>624</v>
       </c>
@@ -46322,17 +45302,10 @@
         <v>14</v>
       </c>
       <c r="F157" s="33">
-        <v>134</v>
-      </c>
-      <c r="G157" s="48">
-        <v>105</v>
-      </c>
-      <c r="H157" s="33">
-        <f t="shared" si="2"/>
         <v>239</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B158" s="33" t="s">
         <v>325</v>
       </c>
@@ -46346,17 +45319,10 @@
         <v>14</v>
       </c>
       <c r="F158" s="33">
-        <v>47</v>
-      </c>
-      <c r="G158" s="48">
-        <v>36</v>
-      </c>
-      <c r="H158" s="33">
-        <f t="shared" si="2"/>
         <v>83</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="168" t="s">
         <v>625</v>
       </c>
@@ -46373,17 +45339,10 @@
         <v>84</v>
       </c>
       <c r="F159" s="50">
-        <v>563</v>
-      </c>
-      <c r="G159" s="168">
-        <v>451</v>
-      </c>
-      <c r="H159" s="50">
-        <f t="shared" si="2"/>
         <v>1014</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B160" s="33" t="s">
         <v>1277</v>
       </c>
@@ -46397,17 +45356,10 @@
         <v>84</v>
       </c>
       <c r="F160" s="33">
-        <v>113</v>
-      </c>
-      <c r="G160" s="48">
-        <v>127</v>
-      </c>
-      <c r="H160" s="33">
-        <f t="shared" si="2"/>
         <v>240</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B161" s="33" t="s">
         <v>628</v>
       </c>
@@ -46421,17 +45373,10 @@
         <v>86</v>
       </c>
       <c r="F161" s="33">
-        <v>97</v>
-      </c>
-      <c r="G161" s="48">
-        <v>73</v>
-      </c>
-      <c r="H161" s="33">
-        <f t="shared" si="2"/>
         <v>170</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B162" s="33" t="s">
         <v>912</v>
       </c>
@@ -46445,17 +45390,10 @@
         <v>84</v>
       </c>
       <c r="F162" s="33">
-        <v>90</v>
-      </c>
-      <c r="G162" s="48">
-        <v>48</v>
-      </c>
-      <c r="H162" s="33">
-        <f t="shared" si="2"/>
         <v>138</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B163" s="33" t="s">
         <v>630</v>
       </c>
@@ -46469,17 +45407,10 @@
         <v>86</v>
       </c>
       <c r="F163" s="33">
-        <v>4</v>
-      </c>
-      <c r="G163" s="48">
-        <v>4</v>
-      </c>
-      <c r="H163" s="33">
-        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="168" t="s">
         <v>13</v>
       </c>
@@ -46495,18 +45426,11 @@
       <c r="E164" s="175" t="s">
         <v>14</v>
       </c>
-      <c r="F164" s="50">
-        <v>175</v>
-      </c>
-      <c r="G164" s="168">
-        <v>175</v>
-      </c>
-      <c r="H164" s="32">
-        <f t="shared" si="2"/>
+      <c r="F164" s="32">
         <v>350</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="168" t="s">
         <v>632</v>
       </c>
@@ -46523,17 +45447,10 @@
         <v>86</v>
       </c>
       <c r="F165" s="50">
-        <v>73</v>
-      </c>
-      <c r="G165" s="168">
-        <v>28</v>
-      </c>
-      <c r="H165" s="50">
-        <f t="shared" si="2"/>
         <v>101</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B166" s="33" t="s">
         <v>634</v>
       </c>
@@ -46547,17 +45464,10 @@
         <v>86</v>
       </c>
       <c r="F166" s="33">
-        <v>61</v>
-      </c>
-      <c r="G166" s="48">
-        <v>47</v>
-      </c>
-      <c r="H166" s="33">
-        <f t="shared" si="2"/>
         <v>108</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B167" s="33" t="s">
         <v>635</v>
       </c>
@@ -46571,17 +45481,10 @@
         <v>86</v>
       </c>
       <c r="F167" s="33">
-        <v>55</v>
-      </c>
-      <c r="G167" s="48">
-        <v>12</v>
-      </c>
-      <c r="H167" s="33">
-        <f t="shared" si="2"/>
         <v>67</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B168" s="33" t="s">
         <v>636</v>
       </c>
@@ -46595,17 +45498,10 @@
         <v>86</v>
       </c>
       <c r="F168" s="33">
-        <v>18</v>
-      </c>
-      <c r="G168" s="48">
-        <v>18</v>
-      </c>
-      <c r="H168" s="33">
-        <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B169" s="33" t="s">
         <v>637</v>
       </c>
@@ -46619,17 +45515,10 @@
         <v>86</v>
       </c>
       <c r="F169" s="33">
-        <v>188</v>
-      </c>
-      <c r="G169" s="48">
-        <v>161</v>
-      </c>
-      <c r="H169" s="33">
-        <f t="shared" si="2"/>
         <v>349</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B170" s="33" t="s">
         <v>638</v>
       </c>
@@ -46643,17 +45532,10 @@
         <v>86</v>
       </c>
       <c r="F170" s="33">
-        <v>40</v>
-      </c>
-      <c r="G170" s="48">
-        <v>35</v>
-      </c>
-      <c r="H170" s="33">
-        <f t="shared" si="2"/>
         <v>75</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B171" s="33" t="s">
         <v>639</v>
       </c>
@@ -46667,17 +45549,10 @@
         <v>86</v>
       </c>
       <c r="F171" s="33">
-        <v>20</v>
-      </c>
-      <c r="G171" s="48">
-        <v>3</v>
-      </c>
-      <c r="H171" s="33">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B172" s="33" t="s">
         <v>640</v>
       </c>
@@ -46691,17 +45566,10 @@
         <v>86</v>
       </c>
       <c r="F172" s="33">
-        <v>2</v>
-      </c>
-      <c r="G172" s="48">
-        <v>3</v>
-      </c>
-      <c r="H172" s="33">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B173" s="33" t="s">
         <v>641</v>
       </c>
@@ -46715,17 +45583,10 @@
         <v>86</v>
       </c>
       <c r="F173" s="33">
-        <v>1</v>
-      </c>
-      <c r="G173" s="48">
-        <v>9</v>
-      </c>
-      <c r="H173" s="33">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B174" s="33" t="s">
         <v>642</v>
       </c>
@@ -46739,17 +45600,10 @@
         <v>86</v>
       </c>
       <c r="F174" s="33">
-        <v>26</v>
-      </c>
-      <c r="G174" s="48">
-        <v>33</v>
-      </c>
-      <c r="H174" s="33">
-        <f t="shared" si="2"/>
         <v>59</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B175" s="33" t="s">
         <v>643</v>
       </c>
@@ -46763,17 +45617,10 @@
         <v>86</v>
       </c>
       <c r="F175" s="33">
-        <v>30</v>
-      </c>
-      <c r="G175" s="48">
-        <v>35</v>
-      </c>
-      <c r="H175" s="33">
-        <f t="shared" si="2"/>
         <v>65</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B176" s="33" t="s">
         <v>644</v>
       </c>
@@ -46787,17 +45634,10 @@
         <v>86</v>
       </c>
       <c r="F176" s="33">
-        <v>24</v>
-      </c>
-      <c r="G176" s="48">
-        <v>40</v>
-      </c>
-      <c r="H176" s="33">
-        <f t="shared" si="2"/>
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B177" s="33" t="s">
         <v>645</v>
       </c>
@@ -46811,17 +45651,10 @@
         <v>86</v>
       </c>
       <c r="F177" s="33">
-        <v>86</v>
-      </c>
-      <c r="G177" s="48">
-        <v>54</v>
-      </c>
-      <c r="H177" s="33">
-        <f t="shared" si="2"/>
         <v>140</v>
       </c>
     </row>
-    <row r="178" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B178" s="33" t="s">
         <v>646</v>
       </c>
@@ -46835,17 +45668,10 @@
         <v>86</v>
       </c>
       <c r="F178" s="33">
-        <v>102</v>
-      </c>
-      <c r="G178" s="48">
-        <v>24</v>
-      </c>
-      <c r="H178" s="33">
-        <f t="shared" si="2"/>
         <v>126</v>
       </c>
     </row>
-    <row r="179" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B179" s="33" t="s">
         <v>356</v>
       </c>
@@ -46859,17 +45685,10 @@
         <v>86</v>
       </c>
       <c r="F179" s="33">
-        <v>107</v>
-      </c>
-      <c r="G179" s="48">
-        <v>196</v>
-      </c>
-      <c r="H179" s="33">
-        <f t="shared" si="2"/>
         <v>303</v>
       </c>
     </row>
-    <row r="180" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B180" s="33" t="s">
         <v>647</v>
       </c>
@@ -46883,17 +45702,10 @@
         <v>86</v>
       </c>
       <c r="F180" s="33">
-        <v>35</v>
-      </c>
-      <c r="G180" s="48">
-        <v>72</v>
-      </c>
-      <c r="H180" s="33">
-        <f t="shared" si="2"/>
         <v>107</v>
       </c>
     </row>
-    <row r="181" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B181" s="33" t="s">
         <v>648</v>
       </c>
@@ -46907,17 +45719,10 @@
         <v>86</v>
       </c>
       <c r="F181" s="33">
-        <v>3</v>
-      </c>
-      <c r="G181" s="48">
-        <v>2</v>
-      </c>
-      <c r="H181" s="33">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B182" s="33" t="s">
         <v>649</v>
       </c>
@@ -46931,17 +45736,10 @@
         <v>86</v>
       </c>
       <c r="F182" s="33">
-        <v>297</v>
-      </c>
-      <c r="G182" s="48">
-        <v>154</v>
-      </c>
-      <c r="H182" s="33">
-        <f t="shared" si="2"/>
         <v>451</v>
       </c>
     </row>
-    <row r="183" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B183" s="33" t="s">
         <v>650</v>
       </c>
@@ -46955,17 +45753,10 @@
         <v>86</v>
       </c>
       <c r="F183" s="33">
-        <v>2</v>
-      </c>
-      <c r="G183" s="48">
-        <v>37</v>
-      </c>
-      <c r="H183" s="33">
-        <f t="shared" si="2"/>
         <v>39</v>
       </c>
     </row>
-    <row r="184" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B184" s="33" t="s">
         <v>651</v>
       </c>
@@ -46978,16 +45769,11 @@
       <c r="E184" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="F184" s="33"/>
-      <c r="G184" s="48">
+      <c r="F184" s="33">
         <v>4</v>
       </c>
-      <c r="H184" s="33">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="185" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="185" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B185" s="33" t="s">
         <v>652</v>
       </c>
@@ -47001,17 +45787,10 @@
         <v>86</v>
       </c>
       <c r="F185" s="33">
-        <v>68</v>
-      </c>
-      <c r="G185" s="48">
-        <v>35</v>
-      </c>
-      <c r="H185" s="33">
-        <f t="shared" si="2"/>
         <v>103</v>
       </c>
     </row>
-    <row r="186" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B186" s="33" t="s">
         <v>913</v>
       </c>
@@ -47025,17 +45804,10 @@
         <v>86</v>
       </c>
       <c r="F186" s="33">
-        <v>163</v>
-      </c>
-      <c r="G186" s="48">
-        <v>189</v>
-      </c>
-      <c r="H186" s="33">
-        <f t="shared" si="2"/>
         <v>352</v>
       </c>
     </row>
-    <row r="187" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B187" s="33" t="s">
         <v>914</v>
       </c>
@@ -47049,17 +45821,10 @@
         <v>86</v>
       </c>
       <c r="F187" s="33">
-        <v>117</v>
-      </c>
-      <c r="G187" s="48">
-        <v>29</v>
-      </c>
-      <c r="H187" s="33">
-        <f t="shared" si="2"/>
         <v>146</v>
       </c>
     </row>
-    <row r="188" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B188" s="33" t="s">
         <v>915</v>
       </c>
@@ -47073,17 +45838,10 @@
         <v>86</v>
       </c>
       <c r="F188" s="33">
-        <v>296</v>
-      </c>
-      <c r="G188" s="48">
-        <v>237</v>
-      </c>
-      <c r="H188" s="33">
-        <f t="shared" si="2"/>
         <v>533</v>
       </c>
     </row>
-    <row r="189" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B189" s="33" t="s">
         <v>916</v>
       </c>
@@ -47097,17 +45855,10 @@
         <v>86</v>
       </c>
       <c r="F189" s="33">
-        <v>61</v>
-      </c>
-      <c r="G189" s="48">
-        <v>84</v>
-      </c>
-      <c r="H189" s="33">
-        <f t="shared" si="2"/>
         <v>145</v>
       </c>
     </row>
-    <row r="190" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B190" s="33" t="s">
         <v>917</v>
       </c>
@@ -47121,17 +45872,10 @@
         <v>86</v>
       </c>
       <c r="F190" s="33">
-        <v>26</v>
-      </c>
-      <c r="G190" s="48">
-        <v>13</v>
-      </c>
-      <c r="H190" s="33">
-        <f t="shared" si="2"/>
         <v>39</v>
       </c>
     </row>
-    <row r="191" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B191" s="33" t="s">
         <v>659</v>
       </c>
@@ -47145,17 +45889,10 @@
         <v>86</v>
       </c>
       <c r="F191" s="33">
-        <v>12</v>
-      </c>
-      <c r="G191" s="48">
-        <v>24</v>
-      </c>
-      <c r="H191" s="33">
-        <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B192" s="33" t="s">
         <v>660</v>
       </c>
@@ -47169,17 +45906,10 @@
         <v>86</v>
       </c>
       <c r="F192" s="33">
-        <v>1</v>
-      </c>
-      <c r="G192" s="48">
-        <v>1</v>
-      </c>
-      <c r="H192" s="33">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B193" s="33" t="s">
         <v>661</v>
       </c>
@@ -47192,16 +45922,11 @@
       <c r="E193" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="F193" s="33"/>
-      <c r="G193" s="48">
+      <c r="F193" s="33">
         <v>6</v>
       </c>
-      <c r="H193" s="33">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B194" s="33" t="s">
         <v>662</v>
       </c>
@@ -47215,17 +45940,10 @@
         <v>86</v>
       </c>
       <c r="F194" s="33">
-        <v>7</v>
-      </c>
-      <c r="G194" s="48">
-        <v>28</v>
-      </c>
-      <c r="H194" s="33">
-        <f t="shared" si="2"/>
         <v>35</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B195" s="33" t="s">
         <v>663</v>
       </c>
@@ -47238,16 +45956,11 @@
       <c r="E195" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="F195" s="33"/>
-      <c r="G195" s="48">
+      <c r="F195" s="33">
         <v>2</v>
       </c>
-      <c r="H195" s="33">
-        <f t="shared" ref="H195:H205" si="3">F195+G195</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="196" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B196" s="33" t="s">
         <v>664</v>
       </c>
@@ -47261,17 +45974,10 @@
         <v>86</v>
       </c>
       <c r="F196" s="33">
-        <v>13</v>
-      </c>
-      <c r="G196" s="48">
-        <v>32</v>
-      </c>
-      <c r="H196" s="33">
-        <f t="shared" si="3"/>
         <v>45</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B197" s="33" t="s">
         <v>665</v>
       </c>
@@ -47285,17 +45991,10 @@
         <v>86</v>
       </c>
       <c r="F197" s="33">
-        <v>11</v>
-      </c>
-      <c r="G197" s="48">
-        <v>9</v>
-      </c>
-      <c r="H197" s="33">
-        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B198" s="33" t="s">
         <v>666</v>
       </c>
@@ -47309,17 +46008,10 @@
         <v>86</v>
       </c>
       <c r="F198" s="33">
-        <v>61</v>
-      </c>
-      <c r="G198" s="48">
-        <v>96</v>
-      </c>
-      <c r="H198" s="33">
-        <f t="shared" si="3"/>
         <v>157</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B199" s="33" t="s">
         <v>667</v>
       </c>
@@ -47333,17 +46025,10 @@
         <v>86</v>
       </c>
       <c r="F199" s="33">
-        <v>116</v>
-      </c>
-      <c r="G199" s="48">
-        <v>99</v>
-      </c>
-      <c r="H199" s="33">
-        <f t="shared" si="3"/>
         <v>215</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B200" s="33" t="s">
         <v>668</v>
       </c>
@@ -47357,17 +46042,10 @@
         <v>86</v>
       </c>
       <c r="F200" s="33">
-        <v>13</v>
-      </c>
-      <c r="G200" s="48">
-        <v>14</v>
-      </c>
-      <c r="H200" s="33">
-        <f t="shared" si="3"/>
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B201" s="33" t="s">
         <v>669</v>
       </c>
@@ -47381,17 +46059,10 @@
         <v>86</v>
       </c>
       <c r="F201" s="33">
-        <v>37</v>
-      </c>
-      <c r="G201" s="48">
-        <v>21</v>
-      </c>
-      <c r="H201" s="33">
-        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="168" t="s">
         <v>670</v>
       </c>
@@ -47408,17 +46079,10 @@
         <v>84</v>
       </c>
       <c r="F202" s="50">
-        <v>3</v>
-      </c>
-      <c r="G202" s="168">
-        <v>3</v>
-      </c>
-      <c r="H202" s="50">
-        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="37"/>
       <c r="B203" s="33" t="s">
         <v>672</v>
@@ -47432,16 +46096,11 @@
       <c r="E203" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F203" s="33"/>
-      <c r="G203" s="37">
+      <c r="F203" s="33">
         <v>1</v>
       </c>
-      <c r="H203" s="33">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="37"/>
       <c r="B204" s="33" t="s">
         <v>673</v>
@@ -47456,17 +46115,10 @@
         <v>84</v>
       </c>
       <c r="F204" s="33">
-        <v>16</v>
-      </c>
-      <c r="G204" s="37">
-        <v>38</v>
-      </c>
-      <c r="H204" s="33">
-        <f t="shared" si="3"/>
         <v>54</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="53"/>
       <c r="B205" s="35" t="s">
         <v>674</v>
@@ -47480,19 +46132,12 @@
       <c r="E205" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F205" s="35">
-        <v>7</v>
-      </c>
-      <c r="G205" s="53">
-        <v>13</v>
-      </c>
-      <c r="H205" s="33">
-        <f t="shared" si="3"/>
+      <c r="F205" s="33">
         <v>20</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H206" s="168"/>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F206" s="168"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -47503,7 +46148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5152F6-972D-7D4C-9BE9-115020DCE41E}">
   <dimension ref="A1:H206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>

</xml_diff>

<commit_message>
Replaced all null values with zeroes (0).
</commit_message>
<xml_diff>
--- a/CA 1900-2020 Project.xlsx
+++ b/CA 1900-2020 Project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9510D0A-84DB-1948-B04A-62198A076083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70855BA0-721D-4340-A9D6-60439BEF96CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y1900" sheetId="1" r:id="rId1"/>
@@ -37,13 +37,13 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="40" r:id="rId19"/>
-    <pivotCache cacheId="41" r:id="rId20"/>
-    <pivotCache cacheId="42" r:id="rId21"/>
-    <pivotCache cacheId="43" r:id="rId22"/>
-    <pivotCache cacheId="44" r:id="rId23"/>
-    <pivotCache cacheId="45" r:id="rId24"/>
-    <pivotCache cacheId="46" r:id="rId25"/>
+    <pivotCache cacheId="47" r:id="rId19"/>
+    <pivotCache cacheId="48" r:id="rId20"/>
+    <pivotCache cacheId="49" r:id="rId21"/>
+    <pivotCache cacheId="50" r:id="rId22"/>
+    <pivotCache cacheId="51" r:id="rId23"/>
+    <pivotCache cacheId="52" r:id="rId24"/>
+    <pivotCache cacheId="53" r:id="rId25"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -13525,7 +13525,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="47" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G2:H11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13595,7 +13595,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F71FD943-D8DE-B04D-A293-4F8A349850E4}" name="PivotTable3" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F71FD943-D8DE-B04D-A293-4F8A349850E4}" name="PivotTable3" cacheId="48" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:C12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -13693,7 +13693,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F5CE638-D57B-2D45-A776-7B74F40C3272}" name="PivotTable1" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F5CE638-D57B-2D45-A776-7B74F40C3272}" name="PivotTable1" cacheId="49" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H2:I17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -13832,7 +13832,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA77B427-30EE-2D4E-AF9F-FB74689F53BA}" name="PivotTable2" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA77B427-30EE-2D4E-AF9F-FB74689F53BA}" name="PivotTable2" cacheId="53" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N2:O17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -13970,7 +13970,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0980F33B-844F-CB44-945E-9EC5C1BFF35C}" name="PivotTable6" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0980F33B-844F-CB44-945E-9EC5C1BFF35C}" name="PivotTable6" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E2:F17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -14100,7 +14100,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DCBFB610-686F-5F40-B4FD-EF02A31BB584}" name="PivotTable5" cacheId="44" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DCBFB610-686F-5F40-B4FD-EF02A31BB584}" name="PivotTable5" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K2:L17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -14236,7 +14236,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7BB1F9D-9A4F-BA48-A5D5-2977DEB5B29A}" name="PivotTable4" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7BB1F9D-9A4F-BA48-A5D5-2977DEB5B29A}" name="PivotTable4" cacheId="50" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="Q2:R17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -14694,8 +14694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A11" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15663,7 +15663,7 @@
         <v>83</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F38" s="8">
         <f>2588-SUM(F37)</f>
@@ -16071,8 +16071,8 @@
   <dimension ref="A1:H282"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="176" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G279" sqref="G279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16127,7 +16127,9 @@
       <c r="E2" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="33"/>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="33" t="s">
@@ -16142,7 +16144,9 @@
       <c r="E3" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="33"/>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="33" t="s">
@@ -16191,7 +16195,9 @@
       <c r="E6" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="33" t="s">
@@ -16325,7 +16331,9 @@
       <c r="E14" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="33"/>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="33" t="s">
@@ -16340,7 +16348,9 @@
       <c r="E15" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="33"/>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="33" t="s">
@@ -16355,7 +16365,9 @@
       <c r="E16" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="33"/>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="33" t="s">
@@ -16370,7 +16382,9 @@
       <c r="E17" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="33" t="s">
@@ -16521,7 +16535,9 @@
       <c r="E26" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="33"/>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="33" t="s">
@@ -16553,7 +16569,9 @@
       <c r="E28" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="33"/>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="33" t="s">
@@ -16585,7 +16603,9 @@
       <c r="E30" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F30" s="33"/>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="33" t="s">
@@ -16651,7 +16671,9 @@
       <c r="E34" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F34" s="33"/>
+      <c r="F34" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="33" t="s">
@@ -16683,7 +16705,9 @@
       <c r="E36" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="33"/>
+      <c r="F36" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="33" t="s">
@@ -16698,7 +16722,9 @@
       <c r="E37" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="33"/>
+      <c r="F37" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="33" t="s">
@@ -16713,7 +16739,9 @@
       <c r="E38" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="33"/>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="33" t="s">
@@ -16728,7 +16756,9 @@
       <c r="E39" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F39" s="33"/>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="33" t="s">
@@ -16760,7 +16790,9 @@
       <c r="E41" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="33"/>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="33" t="s">
@@ -16877,7 +16909,9 @@
       <c r="E48" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F48" s="33"/>
+      <c r="F48" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="33" t="s">
@@ -16926,7 +16960,9 @@
       <c r="E51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F51" s="33"/>
+      <c r="F51" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="s">
@@ -16941,7 +16977,9 @@
       <c r="E52" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F52" s="33"/>
+      <c r="F52" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="33" t="s">
@@ -17984,7 +18022,9 @@
       <c r="E113" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F113" s="33"/>
+      <c r="F113" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B114" s="33" t="s">
@@ -18368,7 +18408,9 @@
       <c r="E135" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="F135" s="33"/>
+      <c r="F135" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B136" s="33" t="s">
@@ -18400,7 +18442,9 @@
       <c r="E137" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="F137" s="33"/>
+      <c r="F137" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="33" t="s">
@@ -19870,7 +19914,9 @@
       <c r="E222" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F222" s="33"/>
+      <c r="F222" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B223" s="33" t="s">
@@ -19937,7 +19983,9 @@
       <c r="E226" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F226" s="35"/>
+      <c r="F226" s="35">
+        <v>0</v>
+      </c>
     </row>
     <row r="227" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="48" t="s">
@@ -20858,7 +20906,9 @@
       <c r="E279" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="F279" s="95"/>
+      <c r="F279" s="95">
+        <v>0</v>
+      </c>
     </row>
     <row r="280" spans="1:6" s="100" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B280" s="106" t="s">
@@ -20958,9 +21008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11268065-042F-7744-9FAD-BCB8A8758450}">
   <dimension ref="A1:H283"/>
   <sheetViews>
-    <sheetView zoomScale="167" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G277" sqref="G277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21015,7 +21065,9 @@
       <c r="E2" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="33"/>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="33"/>
@@ -21157,7 +21209,9 @@
       <c r="E10" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="33"/>
@@ -21173,7 +21227,9 @@
       <c r="E11" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="33"/>
@@ -21297,7 +21353,9 @@
       <c r="E18" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="33"/>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="33"/>
@@ -21313,7 +21371,9 @@
       <c r="E19" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="33"/>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="33"/>
@@ -21365,7 +21425,9 @@
       <c r="E22" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="33"/>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="33"/>
@@ -21435,7 +21497,9 @@
       <c r="E26" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="33"/>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="33"/>
@@ -21541,7 +21605,9 @@
       <c r="E32" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="33"/>
@@ -22621,7 +22687,9 @@
       <c r="E92" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F92" s="33"/>
+      <c r="F92" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="33"/>
@@ -24651,7 +24719,9 @@
       <c r="E204" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F204" s="33"/>
+      <c r="F204" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="35"/>
@@ -24705,7 +24775,9 @@
       <c r="E207" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F207" s="33"/>
+      <c r="F207" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="33"/>
@@ -24721,7 +24793,9 @@
       <c r="E208" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F208" s="33"/>
+      <c r="F208" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="33"/>
@@ -24809,7 +24883,9 @@
       <c r="E213" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F213" s="33"/>
+      <c r="F213" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="33"/>
@@ -24861,7 +24937,9 @@
       <c r="E216" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F216" s="33"/>
+      <c r="F216" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="35"/>
@@ -24877,7 +24955,9 @@
       <c r="E217" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="F217" s="35"/>
+      <c r="F217" s="35">
+        <v>0</v>
+      </c>
     </row>
     <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="33" t="s">
@@ -25949,7 +26029,9 @@
       <c r="E276" s="100" t="s">
         <v>86</v>
       </c>
-      <c r="F276" s="95"/>
+      <c r="F276" s="95">
+        <v>0</v>
+      </c>
     </row>
     <row r="277" spans="1:6" s="100" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A277" s="95"/>
@@ -33183,9 +33265,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B2E49A-556D-F34D-9F51-F7E75AC7C46E}">
   <dimension ref="A1:J205"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C121" sqref="C121"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39099,8 +39181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E69982-BF0E-F041-A45E-74DA75E5B4F6}">
   <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
@@ -42545,8 +42627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5E015A-69B3-E449-BA8B-148C187E74C0}">
   <dimension ref="A1:H206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -46149,9 +46231,9 @@
   <dimension ref="A1:H206"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>
+      <selection pane="bottomLeft" activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46242,7 +46324,9 @@
       <c r="E4" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="33"/>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33"/>
@@ -46384,7 +46468,9 @@
       <c r="E12" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="33"/>
@@ -46400,7 +46486,9 @@
       <c r="E13" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="33"/>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="33"/>
@@ -46560,7 +46648,9 @@
       <c r="E22" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="33"/>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="33"/>
@@ -46576,7 +46666,9 @@
       <c r="E23" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="33"/>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="33"/>
@@ -48166,7 +48258,9 @@
       <c r="E111" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F111" s="33"/>
+      <c r="F111" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="33"/>
@@ -48454,7 +48548,9 @@
       <c r="E127" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F127" s="33"/>
+      <c r="F127" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="33"/>
@@ -48814,7 +48910,9 @@
       <c r="E147" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F147" s="35"/>
+      <c r="F147" s="35">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="33" t="s">
@@ -48942,7 +49040,9 @@
       <c r="E154" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F154" s="33"/>
+      <c r="F154" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="35"/>
@@ -49832,7 +49932,9 @@
       <c r="E203" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="F203" s="50"/>
+      <c r="F203" s="50">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="33"/>
@@ -50270,9 +50372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G200" sqref="G200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50488,7 +50590,9 @@
       <c r="E11" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="22"/>
+      <c r="F11" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="33"/>
@@ -50612,7 +50716,9 @@
       <c r="E18" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="34"/>
@@ -50646,7 +50752,9 @@
       <c r="E20" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="22"/>
+      <c r="F20" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="33"/>
@@ -50680,7 +50788,9 @@
       <c r="E22" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="22"/>
+      <c r="F22" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="33"/>
@@ -50768,7 +50878,9 @@
       <c r="E27" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="22"/>
+      <c r="F27" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="33"/>
@@ -50856,7 +50968,9 @@
       <c r="E32" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="22"/>
+      <c r="F32" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="33"/>
@@ -50872,7 +50986,9 @@
       <c r="E33" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="22"/>
+      <c r="F33" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="33"/>
@@ -50888,7 +51004,9 @@
       <c r="E34" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F34" s="22"/>
+      <c r="F34" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="33"/>
@@ -50922,7 +51040,9 @@
       <c r="E36" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="22"/>
+      <c r="F36" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="33"/>
@@ -51010,7 +51130,9 @@
       <c r="E41" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="22"/>
+      <c r="F41" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="33"/>
@@ -51044,7 +51166,9 @@
       <c r="E43" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F43" s="22"/>
+      <c r="F43" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="33"/>
@@ -51078,7 +51202,9 @@
       <c r="E45" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F45" s="22"/>
+      <c r="F45" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="33"/>
@@ -51094,7 +51220,9 @@
       <c r="E46" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F46" s="22"/>
+      <c r="F46" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="33"/>
@@ -51110,7 +51238,9 @@
       <c r="E47" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F47" s="22"/>
+      <c r="F47" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="33"/>
@@ -51126,7 +51256,9 @@
       <c r="E48" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F48" s="22"/>
+      <c r="F48" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="33"/>
@@ -51160,7 +51292,9 @@
       <c r="E50" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F50" s="22"/>
+      <c r="F50" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="33"/>
@@ -51194,7 +51328,9 @@
       <c r="E52" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F52" s="22"/>
+      <c r="F52" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="33"/>
@@ -51210,7 +51346,9 @@
       <c r="E53" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F53" s="22"/>
+      <c r="F53" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="33"/>
@@ -51226,7 +51364,9 @@
       <c r="E54" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F54" s="22"/>
+      <c r="F54" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="35"/>
@@ -52566,7 +52706,9 @@
       <c r="E128" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F128" s="22"/>
+      <c r="F128" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="33"/>
@@ -52600,7 +52742,9 @@
       <c r="E130" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F130" s="22"/>
+      <c r="F130" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="33"/>
@@ -53868,7 +54012,9 @@
       <c r="E200" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F200" s="22"/>
+      <c r="F200" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="35"/>
@@ -54899,9 +55045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E890A69B-E139-B34C-9916-D83CF01530C6}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C143" sqref="C143"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F196" sqref="F196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -55083,7 +55229,9 @@
       <c r="E9" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="33"/>
@@ -55261,7 +55409,9 @@
       <c r="E19" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="33"/>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="33"/>
@@ -55331,7 +55481,9 @@
       <c r="E23" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="33"/>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="33"/>
@@ -55401,7 +55553,9 @@
       <c r="E27" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="33"/>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="33"/>
@@ -55453,7 +55607,9 @@
       <c r="E30" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F30" s="33"/>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="33"/>
@@ -55469,7 +55625,9 @@
       <c r="E31" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="33"/>
@@ -55503,7 +55661,9 @@
       <c r="E33" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="33"/>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="33"/>
@@ -55591,7 +55751,9 @@
       <c r="E38" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="33"/>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="33"/>
@@ -55625,7 +55787,9 @@
       <c r="E40" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="33"/>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="33"/>
@@ -55659,7 +55823,9 @@
       <c r="E42" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F42" s="33"/>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="33"/>
@@ -55675,7 +55841,9 @@
       <c r="E43" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F43" s="33"/>
+      <c r="F43" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="33"/>
@@ -55691,7 +55859,9 @@
       <c r="E44" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="F44" s="33"/>
+      <c r="F44" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="33"/>
@@ -55707,7 +55877,9 @@
       <c r="E45" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F45" s="33"/>
+      <c r="F45" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="33"/>
@@ -55723,7 +55895,9 @@
       <c r="E46" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F46" s="33"/>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="33"/>
@@ -55757,7 +55931,9 @@
       <c r="E48" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F48" s="33"/>
+      <c r="F48" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="33"/>
@@ -55773,7 +55949,9 @@
       <c r="E49" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="F49" s="33"/>
+      <c r="F49" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="33"/>
@@ -57311,7 +57489,9 @@
       <c r="E134" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F134" s="33"/>
+      <c r="F134" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="33"/>
@@ -58433,7 +58613,9 @@
       <c r="E196" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="F196" s="33"/>
+      <c r="F196" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="35"/>

</xml_diff>

<commit_message>
Reclassified anemias as "other chronic," reclassified blood disorders as "other chronic" inn ccb_cause_to_100 sheet.
</commit_message>
<xml_diff>
--- a/CA 1900-2020 Project.xlsx
+++ b/CA 1900-2020 Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA97BA5-1326-6B4D-9557-D9F7AACA5B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D32CE9-7AE3-914D-BAE2-E78BACC00E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y1900" sheetId="1" r:id="rId1"/>
@@ -28742,9 +28742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -30102,8 +30102,8 @@
   <dimension ref="A1:H256"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C187" sqref="C187"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32175,13 +32175,13 @@
         <v>271</v>
       </c>
       <c r="C114" s="75" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D114" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F114" s="27">
         <v>179</v>
@@ -34788,8 +34788,8 @@
   <dimension ref="A1:H282"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -36803,13 +36803,13 @@
         <v>774</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D117" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E117" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F117" s="27">
         <v>38</v>
@@ -36820,13 +36820,13 @@
         <v>775</v>
       </c>
       <c r="C118" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D118" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E118" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F118" s="27">
         <v>56</v>
@@ -36854,13 +36854,13 @@
         <v>777</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D120" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E120" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F120" s="27">
         <v>55</v>
@@ -39732,8 +39732,8 @@
   <dimension ref="A1:H283"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:F1048576"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -41660,13 +41660,13 @@
         <v>774</v>
       </c>
       <c r="C106" s="85" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F106" s="27">
         <v>12</v>
@@ -41678,13 +41678,13 @@
         <v>775</v>
       </c>
       <c r="C107" s="85" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E107" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F107" s="27">
         <v>80</v>
@@ -41714,13 +41714,13 @@
         <v>777</v>
       </c>
       <c r="C109" s="85" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F109" s="27">
         <v>84</v>
@@ -44900,8 +44900,8 @@
   <dimension ref="A1:P103"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -45576,13 +45576,13 @@
         <v>386</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F33" s="33">
         <v>223</v>
@@ -46916,8 +46916,8 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:F1048576"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -47558,13 +47558,13 @@
         <v>386</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F34" s="43">
         <v>339</v>
@@ -48858,8 +48858,8 @@
   <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:F1048576"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -49480,13 +49480,13 @@
         <v>386</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F33" s="57">
         <v>339</v>
@@ -55852,8 +55852,8 @@
   <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -61776,8 +61776,8 @@
   <dimension ref="A1:H189"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -65234,8 +65234,8 @@
   <dimension ref="A1:H206"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -68845,9 +68845,9 @@
   <dimension ref="A1:H206"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C118" sqref="C118"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -72621,9 +72621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A47E31-AC46-354C-870D-B1B8F3EA8B02}">
   <dimension ref="A1:H231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
@@ -76840,9 +76840,9 @@
   <dimension ref="A1:H284"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
@@ -78834,13 +78834,13 @@
         <v>1466</v>
       </c>
       <c r="C99" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E99" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F99" s="130">
         <v>43</v>
@@ -83597,8 +83597,8 @@
   <dimension ref="A1:H256"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C210" sqref="C210:E210"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -85596,13 +85596,13 @@
         <v>271</v>
       </c>
       <c r="C110" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E110" s="26" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F110" s="113">
         <v>139</v>

</xml_diff>

<commit_message>
Reclassification of alcoholism, liver disease, and certain mental health conditions.
</commit_message>
<xml_diff>
--- a/CA 1900-2020 Project.xlsx
+++ b/CA 1900-2020 Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC882CBC-9EC9-A644-A095-184A6F6889A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101EB078-2B1A-164B-95BE-961CAD7F4CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y1900" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15179" uniqueCount="1730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15179" uniqueCount="1732">
   <si>
     <t>Notes</t>
   </si>
@@ -5290,6 +5290,12 @@
   </si>
   <si>
     <t>Other Neurologic</t>
+  </si>
+  <si>
+    <t>Mental Health</t>
+  </si>
+  <si>
+    <t>Kidney Disease and Diabetes</t>
   </si>
 </sst>
 </file>
@@ -5689,7 +5695,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -6196,10 +6202,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8015,9 +8033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8105,7 +8123,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>1730</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -9553,8 +9571,8 @@
   <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11817,7 +11835,7 @@
         <v>158</v>
       </c>
       <c r="C107" s="25" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D107" s="27" t="s">
         <v>21</v>
@@ -12051,8 +12069,8 @@
       <c r="B118" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="C118" s="25" t="s">
-        <v>5</v>
+      <c r="C118" s="202" t="s">
+        <v>1730</v>
       </c>
       <c r="D118" s="27" t="s">
         <v>5</v>
@@ -12073,7 +12091,7 @@
         <v>986</v>
       </c>
       <c r="C119" s="25" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D119" s="27" t="s">
         <v>14</v>
@@ -12094,7 +12112,7 @@
         <v>5</v>
       </c>
       <c r="C120" s="25" t="s">
-        <v>5</v>
+        <v>1730</v>
       </c>
       <c r="D120" s="27" t="s">
         <v>5</v>
@@ -12115,7 +12133,7 @@
         <v>169</v>
       </c>
       <c r="C121" s="25" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D121" s="27" t="s">
         <v>14</v>
@@ -12136,7 +12154,7 @@
         <v>987</v>
       </c>
       <c r="C122" s="74" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D122" s="29" t="s">
         <v>14</v>
@@ -13467,7 +13485,7 @@
         <v>199</v>
       </c>
       <c r="C185" s="25" t="s">
-        <v>5</v>
+        <v>1030</v>
       </c>
       <c r="D185" s="27" t="s">
         <v>5</v>
@@ -13553,7 +13571,7 @@
         <v>301</v>
       </c>
       <c r="C189" s="72" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D189" s="27" t="s">
         <v>935</v>
@@ -13574,7 +13592,7 @@
         <v>302</v>
       </c>
       <c r="C190" s="72" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D190" s="27" t="s">
         <v>935</v>
@@ -13595,7 +13613,7 @@
         <v>1005</v>
       </c>
       <c r="C191" s="72" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D191" s="27" t="s">
         <v>935</v>
@@ -13616,7 +13634,7 @@
         <v>202</v>
       </c>
       <c r="C192" s="72" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D192" s="27" t="s">
         <v>935</v>
@@ -13637,7 +13655,7 @@
         <v>1006</v>
       </c>
       <c r="C193" s="72" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D193" s="27" t="s">
         <v>935</v>
@@ -15038,8 +15056,8 @@
   <dimension ref="A1:I282"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D203" sqref="D203"/>
+      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C208" sqref="C208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17238,7 +17256,7 @@
         <v>158</v>
       </c>
       <c r="C109" s="27" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D109" s="82" t="s">
         <v>21</v>
@@ -17545,8 +17563,8 @@
       <c r="B124" s="27" t="s">
         <v>778</v>
       </c>
-      <c r="C124" s="27" t="s">
-        <v>5</v>
+      <c r="C124" s="201" t="s">
+        <v>1730</v>
       </c>
       <c r="D124" s="82" t="s">
         <v>5</v>
@@ -17566,7 +17584,7 @@
         <v>777</v>
       </c>
       <c r="C125" s="27" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D125" s="82" t="s">
         <v>14</v>
@@ -17586,7 +17604,7 @@
         <v>5</v>
       </c>
       <c r="C126" s="25" t="s">
-        <v>5</v>
+        <v>1730</v>
       </c>
       <c r="D126" s="27" t="s">
         <v>5</v>
@@ -17606,7 +17624,7 @@
         <v>779</v>
       </c>
       <c r="C127" s="27" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D127" s="82" t="s">
         <v>14</v>
@@ -17627,7 +17645,7 @@
         <v>780</v>
       </c>
       <c r="C128" s="29" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D128" s="84" t="s">
         <v>14</v>
@@ -19149,7 +19167,7 @@
         <v>824</v>
       </c>
       <c r="C203" s="27" t="s">
-        <v>5</v>
+        <v>1030</v>
       </c>
       <c r="D203" s="82" t="s">
         <v>5</v>
@@ -19253,7 +19271,7 @@
         <v>301</v>
       </c>
       <c r="C208" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D208" s="82" t="s">
         <v>935</v>
@@ -19273,7 +19291,7 @@
         <v>828</v>
       </c>
       <c r="C209" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D209" s="82" t="s">
         <v>935</v>
@@ -19293,7 +19311,7 @@
         <v>829</v>
       </c>
       <c r="C210" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D210" s="82" t="s">
         <v>935</v>
@@ -19313,7 +19331,7 @@
         <v>202</v>
       </c>
       <c r="C211" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D211" s="82" t="s">
         <v>935</v>
@@ -20890,8 +20908,8 @@
   <dimension ref="A1:I283"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C191" sqref="C191"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22921,7 +22939,7 @@
         <v>158</v>
       </c>
       <c r="C96" s="89" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D96" s="49" t="s">
         <v>21</v>
@@ -24907,7 +24925,7 @@
         <v>1145</v>
       </c>
       <c r="C190" s="89" t="s">
-        <v>5</v>
+        <v>1030</v>
       </c>
       <c r="D190" s="49" t="s">
         <v>5</v>
@@ -25014,7 +25032,7 @@
         <v>1151</v>
       </c>
       <c r="C195" s="89" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D195" s="49" t="s">
         <v>935</v>
@@ -25035,7 +25053,7 @@
         <v>828</v>
       </c>
       <c r="C196" s="89" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D196" s="49" t="s">
         <v>935</v>
@@ -25056,7 +25074,7 @@
         <v>1152</v>
       </c>
       <c r="C197" s="89" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D197" s="49" t="s">
         <v>935</v>
@@ -25077,7 +25095,7 @@
         <v>1153</v>
       </c>
       <c r="C198" s="89" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D198" s="49" t="s">
         <v>935</v>
@@ -25098,7 +25116,7 @@
         <v>202</v>
       </c>
       <c r="C199" s="89" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D199" s="49" t="s">
         <v>935</v>
@@ -26939,9 +26957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -27385,13 +27403,13 @@
         <v>392</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="F16" s="49" t="s">
         <v>24</v>
@@ -27805,7 +27823,7 @@
         <v>384</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>21</v>
@@ -27902,7 +27920,7 @@
       <c r="B38" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C38" s="201" t="s">
+      <c r="C38" s="200" t="s">
         <v>84</v>
       </c>
       <c r="D38" s="43" t="s">
@@ -27927,7 +27945,7 @@
       <c r="B39" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="201" t="s">
+      <c r="C39" s="200" t="s">
         <v>1728</v>
       </c>
       <c r="D39" s="43" t="s">
@@ -28484,7 +28502,10 @@
         <v>1797</v>
       </c>
       <c r="H61" s="138"/>
-      <c r="I61" s="138"/>
+      <c r="I61" s="138">
+        <f>SUM(G59,G60,G61,G62,G63,G66,G65,G64)</f>
+        <v>15672</v>
+      </c>
     </row>
     <row r="62" spans="1:10" ht="16">
       <c r="A62" s="92"/>
@@ -28689,11 +28710,11 @@
       <c r="B70" s="45" t="s">
         <v>451</v>
       </c>
-      <c r="C70" s="199" t="s">
+      <c r="C70" s="45" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D70" s="199" t="s">
         <v>5</v>
-      </c>
-      <c r="D70" s="45" t="s">
-        <v>1030</v>
       </c>
       <c r="E70" s="45" t="s">
         <v>14</v>
@@ -28763,7 +28784,7 @@
         <v>455</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D73" s="45" t="s">
         <v>935</v>
@@ -28786,7 +28807,7 @@
         <v>456</v>
       </c>
       <c r="C74" s="49" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D74" s="49" t="s">
         <v>935</v>
@@ -28809,7 +28830,7 @@
         <v>457</v>
       </c>
       <c r="C75" s="49" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D75" s="49" t="s">
         <v>935</v>
@@ -28832,7 +28853,7 @@
         <v>458</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D76" s="40" t="s">
         <v>935</v>
@@ -28857,7 +28878,7 @@
         <v>384</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D77" s="43" t="s">
         <v>935</v>
@@ -29537,8 +29558,8 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -29897,13 +29918,13 @@
         <v>392</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="F16" s="49" t="s">
         <v>24</v>
@@ -30302,7 +30323,7 @@
         <v>384</v>
       </c>
       <c r="C35" s="43" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D35" s="43" t="s">
         <v>21</v>
@@ -30391,7 +30412,7 @@
       <c r="B39" s="42" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="201" t="s">
+      <c r="C39" s="200" t="s">
         <v>84</v>
       </c>
       <c r="D39" s="43" t="s">
@@ -30414,7 +30435,7 @@
       <c r="B40" s="42" t="s">
         <v>384</v>
       </c>
-      <c r="C40" s="201" t="s">
+      <c r="C40" s="200" t="s">
         <v>1728</v>
       </c>
       <c r="D40" s="43" t="s">
@@ -31170,11 +31191,11 @@
       <c r="B72" s="40" t="s">
         <v>452</v>
       </c>
-      <c r="C72" s="200" t="s">
+      <c r="C72" s="40" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D72" s="203" t="s">
         <v>5</v>
-      </c>
-      <c r="D72" s="91" t="s">
-        <v>1030</v>
       </c>
       <c r="E72" s="91" t="s">
         <v>14</v>
@@ -31217,7 +31238,7 @@
         <v>455</v>
       </c>
       <c r="C74" s="45" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D74" s="45" t="s">
         <v>935</v>
@@ -31238,7 +31259,7 @@
         <v>456</v>
       </c>
       <c r="C75" s="49" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D75" s="49" t="s">
         <v>935</v>
@@ -31259,7 +31280,7 @@
         <v>457</v>
       </c>
       <c r="C76" s="49" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D76" s="49" t="s">
         <v>935</v>
@@ -31282,7 +31303,7 @@
         <v>384</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D77" s="43" t="s">
         <v>935</v>
@@ -31869,9 +31890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F991E2-CA91-C64F-92DE-133AD8400423}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32207,13 +32228,13 @@
         <v>392</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="D15" s="92" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="E15" s="92" t="s">
-        <v>1028</v>
+        <v>932</v>
       </c>
       <c r="F15" s="49" t="s">
         <v>24</v>
@@ -32612,7 +32633,7 @@
         <v>384</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>21</v>
@@ -32701,7 +32722,7 @@
       <c r="B38" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C38" s="201" t="s">
+      <c r="C38" s="200" t="s">
         <v>84</v>
       </c>
       <c r="D38" s="43" t="s">
@@ -32724,7 +32745,7 @@
       <c r="B39" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="201" t="s">
+      <c r="C39" s="200" t="s">
         <v>1728</v>
       </c>
       <c r="D39" s="43" t="s">
@@ -33480,11 +33501,11 @@
       <c r="B71" s="51" t="s">
         <v>452</v>
       </c>
-      <c r="C71" s="200" t="s">
+      <c r="C71" s="40" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D71" s="203" t="s">
         <v>5</v>
-      </c>
-      <c r="D71" s="91" t="s">
-        <v>1030</v>
       </c>
       <c r="E71" s="91" t="s">
         <v>14</v>
@@ -33527,7 +33548,7 @@
         <v>455</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D73" s="90" t="s">
         <v>935</v>
@@ -33548,7 +33569,7 @@
         <v>456</v>
       </c>
       <c r="C74" s="49" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D74" s="92" t="s">
         <v>935</v>
@@ -33569,7 +33590,7 @@
         <v>457</v>
       </c>
       <c r="C75" s="49" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D75" s="92" t="s">
         <v>935</v>
@@ -33590,7 +33611,7 @@
         <v>458</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D76" s="91" t="s">
         <v>935</v>
@@ -33613,7 +33634,7 @@
         <v>384</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D77" s="43" t="s">
         <v>935</v>
@@ -34239,9 +34260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE00D5B-D363-6A46-AEA9-149824DE4DAC}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -35063,7 +35084,7 @@
         <v>158</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D36" t="s">
         <v>21</v>
@@ -35224,7 +35245,7 @@
         <v>1696</v>
       </c>
       <c r="C43" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D43" t="s">
         <v>935</v>
@@ -35678,7 +35699,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView topLeftCell="B15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -36500,7 +36521,7 @@
         <v>158</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D36" t="s">
         <v>21</v>
@@ -36661,7 +36682,7 @@
         <v>1696</v>
       </c>
       <c r="C43" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D43" t="s">
         <v>935</v>
@@ -37114,8 +37135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="99" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="C9" zoomScale="99" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -37565,9 +37586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B2E49A-556D-F34D-9F51-F7E75AC7C46E}">
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -39165,7 +39186,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="82" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>21</v>
@@ -41527,7 +41548,7 @@
         <v>301</v>
       </c>
       <c r="C125" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D125" s="27" t="s">
         <v>935</v>
@@ -41559,7 +41580,7 @@
         <v>588</v>
       </c>
       <c r="C126" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D126" s="27" t="s">
         <v>935</v>
@@ -41591,7 +41612,7 @@
         <v>589</v>
       </c>
       <c r="C127" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D127" s="27" t="s">
         <v>935</v>
@@ -41619,7 +41640,7 @@
         <v>590</v>
       </c>
       <c r="C128" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D128" s="27" t="s">
         <v>935</v>
@@ -44515,8 +44536,8 @@
   <dimension ref="A1:I189"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -45407,7 +45428,7 @@
         <v>21</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D42" s="27" t="s">
         <v>21</v>
@@ -46908,7 +46929,7 @@
         <v>301</v>
       </c>
       <c r="C113" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D113" s="27" t="s">
         <v>935</v>
@@ -46929,7 +46950,7 @@
         <v>588</v>
       </c>
       <c r="C114" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D114" s="27" t="s">
         <v>935</v>
@@ -46950,7 +46971,7 @@
         <v>590</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D115" s="27" t="s">
         <v>935</v>
@@ -48571,8 +48592,8 @@
   <dimension ref="A1:I206"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -49606,7 +49627,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="82" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>21</v>
@@ -51122,7 +51143,7 @@
         <v>301</v>
       </c>
       <c r="C125" s="81" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D125" s="65" t="s">
         <v>935</v>
@@ -51142,7 +51163,7 @@
         <v>588</v>
       </c>
       <c r="C126" s="81" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D126" s="65" t="s">
         <v>935</v>
@@ -51162,7 +51183,7 @@
         <v>589</v>
       </c>
       <c r="C127" s="81" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D127" s="65" t="s">
         <v>935</v>
@@ -51182,7 +51203,7 @@
         <v>590</v>
       </c>
       <c r="C128" s="81" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D128" s="65" t="s">
         <v>935</v>
@@ -52830,10 +52851,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5152F6-972D-7D4C-9BE9-115020DCE41E}">
   <dimension ref="A1:I206"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -53915,7 +53936,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="82" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>21</v>
@@ -55479,7 +55500,7 @@
         <v>301</v>
       </c>
       <c r="C125" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D125" s="27" t="s">
         <v>935</v>
@@ -55500,7 +55521,7 @@
         <v>588</v>
       </c>
       <c r="C126" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D126" s="27" t="s">
         <v>935</v>
@@ -55521,7 +55542,7 @@
         <v>589</v>
       </c>
       <c r="C127" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D127" s="27" t="s">
         <v>935</v>
@@ -55542,7 +55563,7 @@
         <v>590</v>
       </c>
       <c r="C128" s="82" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D128" s="27" t="s">
         <v>935</v>
@@ -57260,8 +57281,8 @@
   <dimension ref="A1:I231"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
@@ -58449,7 +58470,7 @@
         <v>158</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D56" s="27" t="s">
         <v>21</v>
@@ -60286,7 +60307,7 @@
         <v>1342</v>
       </c>
       <c r="C143" s="78" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D143" s="78" t="s">
         <v>935</v>
@@ -60307,7 +60328,7 @@
         <v>1343</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D144" s="27" t="s">
         <v>935</v>
@@ -60328,7 +60349,7 @@
         <v>589</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D145" s="27" t="s">
         <v>935</v>
@@ -60349,7 +60370,7 @@
         <v>590</v>
       </c>
       <c r="C146" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D146" s="27" t="s">
         <v>935</v>
@@ -62202,9 +62223,9 @@
   <dimension ref="A1:I284"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <selection pane="bottomLeft" activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
@@ -64143,7 +64164,7 @@
         <v>158</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D84" s="27" t="s">
         <v>21</v>
@@ -64606,7 +64627,7 @@
       <c r="B104" s="123" t="s">
         <v>1463</v>
       </c>
-      <c r="C104" s="78" t="s">
+      <c r="C104" s="205" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="78" t="s">
@@ -64629,7 +64650,7 @@
       <c r="B105" s="121" t="s">
         <v>1464</v>
       </c>
-      <c r="C105" s="27" t="s">
+      <c r="C105" s="201" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="27" t="s">
@@ -66133,7 +66154,7 @@
         <v>1603</v>
       </c>
       <c r="C170" s="26" t="s">
-        <v>5</v>
+        <v>1030</v>
       </c>
       <c r="D170" s="26" t="s">
         <v>5</v>
@@ -66319,7 +66340,7 @@
         <v>301</v>
       </c>
       <c r="C178" s="78" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D178" s="78" t="s">
         <v>935</v>
@@ -66342,7 +66363,7 @@
         <v>1518</v>
       </c>
       <c r="C179" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D179" s="27" t="s">
         <v>935</v>
@@ -66365,7 +66386,7 @@
         <v>1519</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D180" s="27" t="s">
         <v>935</v>
@@ -66388,7 +66409,7 @@
         <v>1520</v>
       </c>
       <c r="C181" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D181" s="27" t="s">
         <v>935</v>
@@ -66411,7 +66432,7 @@
         <v>1521</v>
       </c>
       <c r="C182" s="129" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D182" s="130" t="s">
         <v>935</v>
@@ -68762,8 +68783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B2DB03-2EAE-2749-A49C-27038286C702}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -69048,7 +69069,7 @@
         <v>158</v>
       </c>
       <c r="B14" s="108" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="C14" s="108" t="s">
         <v>21</v>
@@ -69348,7 +69369,7 @@
         <v>1249</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>935</v>
@@ -69591,9 +69612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I256"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -71770,7 +71791,7 @@
         <v>158</v>
       </c>
       <c r="C103" s="26" t="s">
-        <v>21</v>
+        <v>1731</v>
       </c>
       <c r="D103" s="26" t="s">
         <v>21</v>
@@ -72004,8 +72025,8 @@
       <c r="B114" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="C114" s="82" t="s">
-        <v>5</v>
+      <c r="C114" s="204" t="s">
+        <v>1730</v>
       </c>
       <c r="D114" s="82" t="s">
         <v>5</v>
@@ -72026,7 +72047,7 @@
         <v>168</v>
       </c>
       <c r="C115" s="82" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D115" s="82" t="s">
         <v>14</v>
@@ -72047,7 +72068,7 @@
         <v>5</v>
       </c>
       <c r="C116" s="82" t="s">
-        <v>5</v>
+        <v>1730</v>
       </c>
       <c r="D116" s="82" t="s">
         <v>5</v>
@@ -72068,7 +72089,7 @@
         <v>169</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D117" s="27" t="s">
         <v>14</v>
@@ -72089,7 +72110,7 @@
         <v>170</v>
       </c>
       <c r="C118" s="29" t="s">
-        <v>14</v>
+        <v>1730</v>
       </c>
       <c r="D118" s="29" t="s">
         <v>14</v>
@@ -73420,7 +73441,7 @@
         <v>199</v>
       </c>
       <c r="C181" s="26" t="s">
-        <v>5</v>
+        <v>1030</v>
       </c>
       <c r="D181" s="26" t="s">
         <v>5</v>
@@ -73485,7 +73506,7 @@
         <v>301</v>
       </c>
       <c r="C184" s="26" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D184" s="26" t="s">
         <v>935</v>
@@ -73506,7 +73527,7 @@
         <v>302</v>
       </c>
       <c r="C185" s="26" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D185" s="26" t="s">
         <v>935</v>
@@ -73527,7 +73548,7 @@
         <v>303</v>
       </c>
       <c r="C186" s="26" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D186" s="26" t="s">
         <v>935</v>
@@ -73548,7 +73569,7 @@
         <v>202</v>
       </c>
       <c r="C187" s="26" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D187" s="26" t="s">
         <v>935</v>
@@ -73569,7 +73590,7 @@
         <v>203</v>
       </c>
       <c r="C188" s="26" t="s">
-        <v>935</v>
+        <v>1731</v>
       </c>
       <c r="D188" s="26" t="s">
         <v>935</v>

</xml_diff>

<commit_message>
Significant changes made to appearences of all graphs in order to make them more presentable for an audience. Legend sizes/fonts, graph dimensions, axis labels and titles, graph titles, etc. were all modified.
</commit_message>
<xml_diff>
--- a/CA 1900-2020 Project.xlsx
+++ b/CA 1900-2020 Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101EB078-2B1A-164B-95BE-961CAD7F4CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E639DB7A-1004-AC4C-9971-2663CF550466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y1900" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="234" r:id="rId22"/>
+    <pivotCache cacheId="0" r:id="rId22"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -6115,6 +6115,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -6198,27 +6219,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -7641,7 +7641,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="234" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H2:I11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -8033,9 +8033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12069,7 +12069,7 @@
       <c r="B118" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="C118" s="202" t="s">
+      <c r="C118" s="174" t="s">
         <v>1730</v>
       </c>
       <c r="D118" s="27" t="s">
@@ -17563,7 +17563,7 @@
       <c r="B124" s="27" t="s">
         <v>778</v>
       </c>
-      <c r="C124" s="201" t="s">
+      <c r="C124" s="173" t="s">
         <v>1730</v>
       </c>
       <c r="D124" s="82" t="s">
@@ -27052,7 +27052,7 @@
       <c r="G3" s="34">
         <v>85</v>
       </c>
-      <c r="H3" s="172"/>
+      <c r="H3" s="179"/>
       <c r="I3" s="138"/>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1">
@@ -27075,20 +27075,20 @@
       <c r="G4" s="36">
         <v>19</v>
       </c>
-      <c r="H4" s="172"/>
+      <c r="H4" s="179"/>
       <c r="I4" s="138"/>
       <c r="L4" s="94" t="s">
         <v>489</v>
       </c>
-      <c r="M4" s="171" t="s">
+      <c r="M4" s="178" t="s">
         <v>490</v>
       </c>
-      <c r="N4" s="171"/>
-      <c r="O4" s="171"/>
-      <c r="P4" s="171"/>
-      <c r="Q4" s="171"/>
-      <c r="R4" s="171"/>
-      <c r="S4" s="171"/>
+      <c r="N4" s="178"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="178"/>
+      <c r="Q4" s="178"/>
+      <c r="R4" s="178"/>
+      <c r="S4" s="178"/>
     </row>
     <row r="5" spans="1:19" ht="16">
       <c r="A5" s="88" t="s">
@@ -27114,13 +27114,13 @@
       </c>
       <c r="H5" s="138"/>
       <c r="I5" s="138"/>
-      <c r="M5" s="171"/>
-      <c r="N5" s="171"/>
-      <c r="O5" s="171"/>
-      <c r="P5" s="171"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="171"/>
-      <c r="S5" s="171"/>
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
+      <c r="O5" s="178"/>
+      <c r="P5" s="178"/>
+      <c r="Q5" s="178"/>
+      <c r="R5" s="178"/>
+      <c r="S5" s="178"/>
     </row>
     <row r="6" spans="1:19" ht="16">
       <c r="A6" s="88" t="s">
@@ -27146,13 +27146,13 @@
       </c>
       <c r="H6" s="138"/>
       <c r="I6" s="138"/>
-      <c r="M6" s="171"/>
-      <c r="N6" s="171"/>
-      <c r="O6" s="171"/>
-      <c r="P6" s="171"/>
-      <c r="Q6" s="171"/>
-      <c r="R6" s="171"/>
-      <c r="S6" s="171"/>
+      <c r="M6" s="178"/>
+      <c r="N6" s="178"/>
+      <c r="O6" s="178"/>
+      <c r="P6" s="178"/>
+      <c r="Q6" s="178"/>
+      <c r="R6" s="178"/>
+      <c r="S6" s="178"/>
     </row>
     <row r="7" spans="1:19" ht="16">
       <c r="A7" s="88" t="s">
@@ -27178,13 +27178,13 @@
       </c>
       <c r="H7" s="138"/>
       <c r="I7" s="138"/>
-      <c r="M7" s="171"/>
-      <c r="N7" s="171"/>
-      <c r="O7" s="171"/>
-      <c r="P7" s="171"/>
-      <c r="Q7" s="171"/>
-      <c r="R7" s="171"/>
-      <c r="S7" s="171"/>
+      <c r="M7" s="178"/>
+      <c r="N7" s="178"/>
+      <c r="O7" s="178"/>
+      <c r="P7" s="178"/>
+      <c r="Q7" s="178"/>
+      <c r="R7" s="178"/>
+      <c r="S7" s="178"/>
     </row>
     <row r="8" spans="1:19" ht="16">
       <c r="A8" s="88" t="s">
@@ -27210,13 +27210,13 @@
       </c>
       <c r="H8" s="138"/>
       <c r="I8" s="138"/>
-      <c r="M8" s="171"/>
-      <c r="N8" s="171"/>
-      <c r="O8" s="171"/>
-      <c r="P8" s="171"/>
-      <c r="Q8" s="171"/>
-      <c r="R8" s="171"/>
-      <c r="S8" s="171"/>
+      <c r="M8" s="178"/>
+      <c r="N8" s="178"/>
+      <c r="O8" s="178"/>
+      <c r="P8" s="178"/>
+      <c r="Q8" s="178"/>
+      <c r="R8" s="178"/>
+      <c r="S8" s="178"/>
     </row>
     <row r="9" spans="1:19" ht="48">
       <c r="A9" s="88" t="s">
@@ -27242,13 +27242,13 @@
       </c>
       <c r="H9" s="138"/>
       <c r="I9" s="138"/>
-      <c r="M9" s="171"/>
-      <c r="N9" s="171"/>
-      <c r="O9" s="171"/>
-      <c r="P9" s="171"/>
-      <c r="Q9" s="171"/>
-      <c r="R9" s="171"/>
-      <c r="S9" s="171"/>
+      <c r="M9" s="178"/>
+      <c r="N9" s="178"/>
+      <c r="O9" s="178"/>
+      <c r="P9" s="178"/>
+      <c r="Q9" s="178"/>
+      <c r="R9" s="178"/>
+      <c r="S9" s="178"/>
     </row>
     <row r="10" spans="1:19" ht="16">
       <c r="A10" s="90" t="s">
@@ -27274,13 +27274,13 @@
       </c>
       <c r="H10" s="138"/>
       <c r="I10" s="138"/>
-      <c r="M10" s="171"/>
-      <c r="N10" s="171"/>
-      <c r="O10" s="171"/>
-      <c r="P10" s="171"/>
-      <c r="Q10" s="171"/>
-      <c r="R10" s="171"/>
-      <c r="S10" s="171"/>
+      <c r="M10" s="178"/>
+      <c r="N10" s="178"/>
+      <c r="O10" s="178"/>
+      <c r="P10" s="178"/>
+      <c r="Q10" s="178"/>
+      <c r="R10" s="178"/>
+      <c r="S10" s="178"/>
     </row>
     <row r="11" spans="1:19" ht="16">
       <c r="A11" s="92"/>
@@ -27920,7 +27920,7 @@
       <c r="B38" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C38" s="200" t="s">
+      <c r="C38" s="172" t="s">
         <v>84</v>
       </c>
       <c r="D38" s="43" t="s">
@@ -27945,7 +27945,7 @@
       <c r="B39" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="200" t="s">
+      <c r="C39" s="172" t="s">
         <v>1728</v>
       </c>
       <c r="D39" s="43" t="s">
@@ -27990,11 +27990,11 @@
       <c r="G40" s="34">
         <v>394</v>
       </c>
-      <c r="I40" s="178">
+      <c r="I40" s="185">
         <f>SUM(G41:G42,G51)</f>
         <v>5828</v>
       </c>
-      <c r="J40" s="173">
+      <c r="J40" s="180">
         <v>5867</v>
       </c>
     </row>
@@ -28018,8 +28018,8 @@
       <c r="G41" s="35">
         <v>3404</v>
       </c>
-      <c r="I41" s="179"/>
-      <c r="J41" s="174"/>
+      <c r="I41" s="186"/>
+      <c r="J41" s="181"/>
     </row>
     <row r="42" spans="1:10" ht="16">
       <c r="A42" s="92"/>
@@ -28041,8 +28041,8 @@
       <c r="G42" s="35">
         <v>408</v>
       </c>
-      <c r="I42" s="179"/>
-      <c r="J42" s="174"/>
+      <c r="I42" s="186"/>
+      <c r="J42" s="181"/>
     </row>
     <row r="43" spans="1:10" ht="16">
       <c r="A43" s="92"/>
@@ -28064,8 +28064,8 @@
       <c r="G43" s="35">
         <v>16543</v>
       </c>
-      <c r="I43" s="179"/>
-      <c r="J43" s="174"/>
+      <c r="I43" s="186"/>
+      <c r="J43" s="181"/>
     </row>
     <row r="44" spans="1:10" ht="16">
       <c r="A44" s="92"/>
@@ -28087,11 +28087,11 @@
       <c r="G44" s="35">
         <v>106</v>
       </c>
-      <c r="I44" s="180">
+      <c r="I44" s="187">
         <f>SUM(G43:G46)</f>
         <v>53585</v>
       </c>
-      <c r="J44" s="176">
+      <c r="J44" s="183">
         <v>53593</v>
       </c>
     </row>
@@ -28115,8 +28115,8 @@
       <c r="G45" s="35">
         <v>8568</v>
       </c>
-      <c r="I45" s="180"/>
-      <c r="J45" s="176"/>
+      <c r="I45" s="187"/>
+      <c r="J45" s="183"/>
     </row>
     <row r="46" spans="1:10" ht="32">
       <c r="A46" s="92"/>
@@ -28138,8 +28138,8 @@
       <c r="G46" s="35">
         <v>28368</v>
       </c>
-      <c r="I46" s="180"/>
-      <c r="J46" s="176"/>
+      <c r="I46" s="187"/>
+      <c r="J46" s="183"/>
     </row>
     <row r="47" spans="1:10" ht="16">
       <c r="A47" s="92"/>
@@ -28161,8 +28161,8 @@
       <c r="G47" s="35">
         <v>120</v>
       </c>
-      <c r="I47" s="180"/>
-      <c r="J47" s="176"/>
+      <c r="I47" s="187"/>
+      <c r="J47" s="183"/>
     </row>
     <row r="48" spans="1:10" ht="16">
       <c r="A48" s="92"/>
@@ -28184,11 +28184,11 @@
       <c r="G48" s="35">
         <v>77</v>
       </c>
-      <c r="I48" s="181">
+      <c r="I48" s="188">
         <f>SUM(G52)</f>
         <v>18185</v>
       </c>
-      <c r="J48" s="175">
+      <c r="J48" s="182">
         <v>18101</v>
       </c>
     </row>
@@ -28212,8 +28212,8 @@
       <c r="G49" s="35">
         <v>3160</v>
       </c>
-      <c r="I49" s="181"/>
-      <c r="J49" s="175"/>
+      <c r="I49" s="188"/>
+      <c r="J49" s="182"/>
     </row>
     <row r="50" spans="1:10" ht="16">
       <c r="A50" s="92"/>
@@ -28235,8 +28235,8 @@
       <c r="G50" s="35">
         <v>7278</v>
       </c>
-      <c r="I50" s="181"/>
-      <c r="J50" s="175"/>
+      <c r="I50" s="188"/>
+      <c r="J50" s="182"/>
     </row>
     <row r="51" spans="1:10" ht="32">
       <c r="A51" s="92"/>
@@ -28258,8 +28258,8 @@
       <c r="G51" s="35">
         <v>2016</v>
       </c>
-      <c r="I51" s="181"/>
-      <c r="J51" s="175"/>
+      <c r="I51" s="188"/>
+      <c r="J51" s="182"/>
     </row>
     <row r="52" spans="1:10" ht="16">
       <c r="A52" s="92"/>
@@ -28281,11 +28281,11 @@
       <c r="G52" s="35">
         <v>18185</v>
       </c>
-      <c r="I52" s="182">
+      <c r="I52" s="189">
         <f>SUM(G40,G47:G50,G53:G56)</f>
         <v>15384</v>
       </c>
-      <c r="J52" s="177">
+      <c r="J52" s="184">
         <v>15424</v>
       </c>
     </row>
@@ -28309,8 +28309,8 @@
       <c r="G53" s="35">
         <v>1629</v>
       </c>
-      <c r="I53" s="182"/>
-      <c r="J53" s="177"/>
+      <c r="I53" s="189"/>
+      <c r="J53" s="184"/>
     </row>
     <row r="54" spans="1:10" ht="16">
       <c r="A54" s="92"/>
@@ -28332,8 +28332,8 @@
       <c r="G54" s="35">
         <v>1407</v>
       </c>
-      <c r="I54" s="182"/>
-      <c r="J54" s="177"/>
+      <c r="I54" s="189"/>
+      <c r="J54" s="184"/>
     </row>
     <row r="55" spans="1:10" ht="16">
       <c r="A55" s="91"/>
@@ -28355,8 +28355,8 @@
       <c r="G55" s="36">
         <v>813</v>
       </c>
-      <c r="I55" s="182"/>
-      <c r="J55" s="177"/>
+      <c r="I55" s="189"/>
+      <c r="J55" s="184"/>
     </row>
     <row r="56" spans="1:10" ht="16">
       <c r="A56" s="88" t="s">
@@ -28380,8 +28380,8 @@
       <c r="G56" s="33">
         <v>506</v>
       </c>
-      <c r="I56" s="182"/>
-      <c r="J56" s="177"/>
+      <c r="I56" s="189"/>
+      <c r="J56" s="184"/>
     </row>
     <row r="57" spans="1:10" ht="16">
       <c r="A57" s="92" t="s">
@@ -28713,7 +28713,7 @@
       <c r="C70" s="45" t="s">
         <v>1030</v>
       </c>
-      <c r="D70" s="199" t="s">
+      <c r="D70" s="171" t="s">
         <v>5</v>
       </c>
       <c r="E70" s="45" t="s">
@@ -30412,7 +30412,7 @@
       <c r="B39" s="42" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="200" t="s">
+      <c r="C39" s="172" t="s">
         <v>84</v>
       </c>
       <c r="D39" s="43" t="s">
@@ -30435,7 +30435,7 @@
       <c r="B40" s="42" t="s">
         <v>384</v>
       </c>
-      <c r="C40" s="200" t="s">
+      <c r="C40" s="172" t="s">
         <v>1728</v>
       </c>
       <c r="D40" s="43" t="s">
@@ -30479,11 +30479,11 @@
       <c r="G41" s="49">
         <v>323</v>
       </c>
-      <c r="I41" s="188">
+      <c r="I41" s="195">
         <f>SUM(G42:G43,G52)</f>
         <v>8202</v>
       </c>
-      <c r="J41" s="183">
+      <c r="J41" s="190">
         <v>8119</v>
       </c>
     </row>
@@ -30507,8 +30507,8 @@
       <c r="G42" s="50">
         <v>4057</v>
       </c>
-      <c r="I42" s="189"/>
-      <c r="J42" s="184"/>
+      <c r="I42" s="196"/>
+      <c r="J42" s="191"/>
     </row>
     <row r="43" spans="1:10" ht="16">
       <c r="A43" s="48"/>
@@ -30530,8 +30530,8 @@
       <c r="G43" s="49">
         <v>412</v>
       </c>
-      <c r="I43" s="189"/>
-      <c r="J43" s="184"/>
+      <c r="I43" s="196"/>
+      <c r="J43" s="191"/>
     </row>
     <row r="44" spans="1:10" ht="16">
       <c r="A44" s="48"/>
@@ -30553,8 +30553,8 @@
       <c r="G44" s="50">
         <v>11005</v>
       </c>
-      <c r="I44" s="189"/>
-      <c r="J44" s="184"/>
+      <c r="I44" s="196"/>
+      <c r="J44" s="191"/>
     </row>
     <row r="45" spans="1:10" ht="16">
       <c r="A45" s="48"/>
@@ -30576,11 +30576,11 @@
       <c r="G45" s="49">
         <v>186</v>
       </c>
-      <c r="I45" s="190">
+      <c r="I45" s="197">
         <f>SUM(G44:G47)</f>
         <v>39663</v>
       </c>
-      <c r="J45" s="185">
+      <c r="J45" s="192">
         <v>39133</v>
       </c>
     </row>
@@ -30604,8 +30604,8 @@
       <c r="G46" s="50">
         <v>6684</v>
       </c>
-      <c r="I46" s="191"/>
-      <c r="J46" s="185"/>
+      <c r="I46" s="198"/>
+      <c r="J46" s="192"/>
     </row>
     <row r="47" spans="1:10" ht="32">
       <c r="A47" s="48"/>
@@ -30627,8 +30627,8 @@
       <c r="G47" s="50">
         <v>21788</v>
       </c>
-      <c r="I47" s="191"/>
-      <c r="J47" s="185"/>
+      <c r="I47" s="198"/>
+      <c r="J47" s="192"/>
     </row>
     <row r="48" spans="1:10" ht="16">
       <c r="A48" s="48"/>
@@ -30650,8 +30650,8 @@
       <c r="G48" s="49">
         <v>115</v>
       </c>
-      <c r="I48" s="191"/>
-      <c r="J48" s="185"/>
+      <c r="I48" s="198"/>
+      <c r="J48" s="192"/>
     </row>
     <row r="49" spans="1:10" ht="16">
       <c r="A49" s="48"/>
@@ -30673,11 +30673,11 @@
       <c r="G49" s="49">
         <v>76</v>
       </c>
-      <c r="I49" s="192">
+      <c r="I49" s="199">
         <f>SUM(G53)</f>
         <v>13662</v>
       </c>
-      <c r="J49" s="186">
+      <c r="J49" s="193">
         <v>13551</v>
       </c>
     </row>
@@ -30701,8 +30701,8 @@
       <c r="G50" s="50">
         <v>4648</v>
       </c>
-      <c r="I50" s="193"/>
-      <c r="J50" s="186"/>
+      <c r="I50" s="200"/>
+      <c r="J50" s="193"/>
     </row>
     <row r="51" spans="1:10" ht="16">
       <c r="A51" s="48"/>
@@ -30724,8 +30724,8 @@
       <c r="G51" s="50">
         <v>9347</v>
       </c>
-      <c r="I51" s="193"/>
-      <c r="J51" s="186"/>
+      <c r="I51" s="200"/>
+      <c r="J51" s="193"/>
     </row>
     <row r="52" spans="1:10" ht="32">
       <c r="A52" s="48"/>
@@ -30747,8 +30747,8 @@
       <c r="G52" s="50">
         <v>3733</v>
       </c>
-      <c r="I52" s="193"/>
-      <c r="J52" s="186"/>
+      <c r="I52" s="200"/>
+      <c r="J52" s="193"/>
     </row>
     <row r="53" spans="1:10" ht="16">
       <c r="A53" s="48"/>
@@ -30770,11 +30770,11 @@
       <c r="G53" s="50">
         <v>13662</v>
       </c>
-      <c r="I53" s="194">
+      <c r="I53" s="201">
         <f>SUM(G41,G48:G51,G54:G57)</f>
         <v>17433</v>
       </c>
-      <c r="J53" s="187">
+      <c r="J53" s="194">
         <v>17182</v>
       </c>
     </row>
@@ -30798,8 +30798,8 @@
       <c r="G54" s="49">
         <v>792</v>
       </c>
-      <c r="I54" s="194"/>
-      <c r="J54" s="187"/>
+      <c r="I54" s="201"/>
+      <c r="J54" s="194"/>
     </row>
     <row r="55" spans="1:10" ht="16">
       <c r="A55" s="48"/>
@@ -30821,8 +30821,8 @@
       <c r="G55" s="49">
         <v>982</v>
       </c>
-      <c r="I55" s="194"/>
-      <c r="J55" s="187"/>
+      <c r="I55" s="201"/>
+      <c r="J55" s="194"/>
     </row>
     <row r="56" spans="1:10" ht="16">
       <c r="A56" s="39"/>
@@ -30844,8 +30844,8 @@
       <c r="G56" s="39">
         <v>704</v>
       </c>
-      <c r="I56" s="194"/>
-      <c r="J56" s="187"/>
+      <c r="I56" s="201"/>
+      <c r="J56" s="194"/>
     </row>
     <row r="57" spans="1:10" ht="16">
       <c r="A57" s="41" t="s">
@@ -30869,8 +30869,8 @@
       <c r="G57" s="43">
         <v>446</v>
       </c>
-      <c r="I57" s="194"/>
-      <c r="J57" s="187"/>
+      <c r="I57" s="201"/>
+      <c r="J57" s="194"/>
     </row>
     <row r="58" spans="1:10" ht="16">
       <c r="A58" s="44" t="s">
@@ -31194,7 +31194,7 @@
       <c r="C72" s="40" t="s">
         <v>1030</v>
       </c>
-      <c r="D72" s="203" t="s">
+      <c r="D72" s="175" t="s">
         <v>5</v>
       </c>
       <c r="E72" s="91" t="s">
@@ -32722,7 +32722,7 @@
       <c r="B38" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C38" s="200" t="s">
+      <c r="C38" s="172" t="s">
         <v>84</v>
       </c>
       <c r="D38" s="43" t="s">
@@ -32745,7 +32745,7 @@
       <c r="B39" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C39" s="200" t="s">
+      <c r="C39" s="172" t="s">
         <v>1728</v>
       </c>
       <c r="D39" s="43" t="s">
@@ -32789,11 +32789,11 @@
       <c r="G40" s="64">
         <v>368</v>
       </c>
-      <c r="I40" s="188">
+      <c r="I40" s="195">
         <f>SUM(G41:G42,G51)</f>
         <v>11856</v>
       </c>
-      <c r="J40" s="195">
+      <c r="J40" s="202">
         <v>11817</v>
       </c>
     </row>
@@ -32817,8 +32817,8 @@
       <c r="G41" s="150">
         <v>5442</v>
       </c>
-      <c r="I41" s="189"/>
-      <c r="J41" s="196"/>
+      <c r="I41" s="196"/>
+      <c r="J41" s="203"/>
     </row>
     <row r="42" spans="1:10" ht="16">
       <c r="A42" s="26"/>
@@ -32840,8 +32840,8 @@
       <c r="G42" s="64">
         <v>903</v>
       </c>
-      <c r="I42" s="189"/>
-      <c r="J42" s="196"/>
+      <c r="I42" s="196"/>
+      <c r="J42" s="203"/>
     </row>
     <row r="43" spans="1:10" ht="16">
       <c r="A43" s="26"/>
@@ -32863,8 +32863,8 @@
       <c r="G43" s="150">
         <v>9839</v>
       </c>
-      <c r="I43" s="189"/>
-      <c r="J43" s="196"/>
+      <c r="I43" s="196"/>
+      <c r="J43" s="203"/>
     </row>
     <row r="44" spans="1:10" ht="16">
       <c r="A44" s="26"/>
@@ -32886,11 +32886,11 @@
       <c r="G44" s="64">
         <v>160</v>
       </c>
-      <c r="I44" s="190">
+      <c r="I44" s="197">
         <f>SUM(G43:G46)</f>
         <v>37465</v>
       </c>
-      <c r="J44" s="197">
+      <c r="J44" s="204">
         <v>37099</v>
       </c>
     </row>
@@ -32914,8 +32914,8 @@
       <c r="G45" s="150">
         <v>7321</v>
       </c>
-      <c r="I45" s="191"/>
-      <c r="J45" s="197"/>
+      <c r="I45" s="198"/>
+      <c r="J45" s="204"/>
     </row>
     <row r="46" spans="1:10" ht="32">
       <c r="A46" s="26"/>
@@ -32937,8 +32937,8 @@
       <c r="G46" s="150">
         <v>20145</v>
       </c>
-      <c r="I46" s="191"/>
-      <c r="J46" s="197"/>
+      <c r="I46" s="198"/>
+      <c r="J46" s="204"/>
     </row>
     <row r="47" spans="1:10" ht="16">
       <c r="A47" s="26"/>
@@ -32960,8 +32960,8 @@
       <c r="G47" s="64">
         <v>140</v>
       </c>
-      <c r="I47" s="191"/>
-      <c r="J47" s="197"/>
+      <c r="I47" s="198"/>
+      <c r="J47" s="204"/>
     </row>
     <row r="48" spans="1:10" ht="16">
       <c r="A48" s="26"/>
@@ -32983,11 +32983,11 @@
       <c r="G48" s="64">
         <v>68</v>
       </c>
-      <c r="I48" s="192">
+      <c r="I48" s="199">
         <f>SUM(G52)</f>
         <v>16457</v>
       </c>
-      <c r="J48" s="198">
+      <c r="J48" s="205">
         <v>16331</v>
       </c>
     </row>
@@ -33011,8 +33011,8 @@
       <c r="G49" s="150">
         <v>7615</v>
       </c>
-      <c r="I49" s="193"/>
-      <c r="J49" s="198"/>
+      <c r="I49" s="200"/>
+      <c r="J49" s="205"/>
     </row>
     <row r="50" spans="1:10" ht="16">
       <c r="A50" s="26"/>
@@ -33034,8 +33034,8 @@
       <c r="G50" s="150">
         <v>10546</v>
       </c>
-      <c r="I50" s="193"/>
-      <c r="J50" s="198"/>
+      <c r="I50" s="200"/>
+      <c r="J50" s="205"/>
     </row>
     <row r="51" spans="1:10" ht="32">
       <c r="A51" s="26"/>
@@ -33057,8 +33057,8 @@
       <c r="G51" s="150">
         <v>5511</v>
       </c>
-      <c r="I51" s="193"/>
-      <c r="J51" s="198"/>
+      <c r="I51" s="200"/>
+      <c r="J51" s="205"/>
     </row>
     <row r="52" spans="1:10" ht="16">
       <c r="A52" s="26"/>
@@ -33080,11 +33080,11 @@
       <c r="G52" s="150">
         <v>16457</v>
       </c>
-      <c r="I52" s="194">
+      <c r="I52" s="201">
         <f>SUM(G40,G47:G50,G53:G56)</f>
         <v>21504</v>
       </c>
-      <c r="J52" s="187">
+      <c r="J52" s="194">
         <v>21287</v>
       </c>
     </row>
@@ -33108,8 +33108,8 @@
       <c r="G53" s="64">
         <v>641</v>
       </c>
-      <c r="I53" s="194"/>
-      <c r="J53" s="187"/>
+      <c r="I53" s="201"/>
+      <c r="J53" s="194"/>
     </row>
     <row r="54" spans="1:10" ht="16">
       <c r="A54" s="26"/>
@@ -33131,8 +33131,8 @@
       <c r="G54" s="64">
         <v>902</v>
       </c>
-      <c r="I54" s="194"/>
-      <c r="J54" s="187"/>
+      <c r="I54" s="201"/>
+      <c r="J54" s="194"/>
     </row>
     <row r="55" spans="1:10" ht="16">
       <c r="A55" s="26"/>
@@ -33154,8 +33154,8 @@
       <c r="G55" s="64">
         <v>782</v>
       </c>
-      <c r="I55" s="194"/>
-      <c r="J55" s="187"/>
+      <c r="I55" s="201"/>
+      <c r="J55" s="194"/>
     </row>
     <row r="56" spans="1:10" ht="16">
       <c r="A56" s="57" t="s">
@@ -33179,8 +33179,8 @@
       <c r="G56" s="57">
         <v>442</v>
       </c>
-      <c r="I56" s="194"/>
-      <c r="J56" s="187"/>
+      <c r="I56" s="201"/>
+      <c r="J56" s="194"/>
     </row>
     <row r="57" spans="1:10" ht="16">
       <c r="A57" s="64" t="s">
@@ -33504,7 +33504,7 @@
       <c r="C71" s="40" t="s">
         <v>1030</v>
       </c>
-      <c r="D71" s="203" t="s">
+      <c r="D71" s="175" t="s">
         <v>5</v>
       </c>
       <c r="E71" s="91" t="s">
@@ -34260,7 +34260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE00D5B-D363-6A46-AEA9-149824DE4DAC}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
@@ -37587,7 +37587,7 @@
   <dimension ref="A1:K205"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -44536,7 +44536,7 @@
   <dimension ref="A1:I189"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
@@ -48592,7 +48592,7 @@
   <dimension ref="A1:I206"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -52852,7 +52852,7 @@
   <dimension ref="A1:I206"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
     </sheetView>
@@ -57281,7 +57281,7 @@
   <dimension ref="A1:I231"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
@@ -62223,9 +62223,9 @@
   <dimension ref="A1:I284"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C178" sqref="C178"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
@@ -64627,7 +64627,7 @@
       <c r="B104" s="123" t="s">
         <v>1463</v>
       </c>
-      <c r="C104" s="205" t="s">
+      <c r="C104" s="177" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="78" t="s">
@@ -64650,7 +64650,7 @@
       <c r="B105" s="121" t="s">
         <v>1464</v>
       </c>
-      <c r="C105" s="201" t="s">
+      <c r="C105" s="173" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="27" t="s">
@@ -68776,6 +68776,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -68783,7 +68784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B2DB03-2EAE-2749-A49C-27038286C702}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -69613,8 +69614,8 @@
   <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -72025,7 +72026,7 @@
       <c r="B114" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="C114" s="204" t="s">
+      <c r="C114" s="176" t="s">
         <v>1730</v>
       </c>
       <c r="D114" s="82" t="s">

</xml_diff>

<commit_message>
Two bullet points added to R Markdown description.
</commit_message>
<xml_diff>
--- a/CA 1900-2020 Project.xlsx
+++ b/CA 1900-2020 Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E639DB7A-1004-AC4C-9971-2663CF550466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AA5C6A-BBB5-6C4D-B660-FDAC112F6FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y1900" sheetId="1" r:id="rId1"/>
@@ -6136,6 +6136,24 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -6152,24 +6170,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8033,7 +8033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
@@ -27052,7 +27052,7 @@
       <c r="G3" s="34">
         <v>85</v>
       </c>
-      <c r="H3" s="179"/>
+      <c r="H3" s="185"/>
       <c r="I3" s="138"/>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1">
@@ -27075,20 +27075,20 @@
       <c r="G4" s="36">
         <v>19</v>
       </c>
-      <c r="H4" s="179"/>
+      <c r="H4" s="185"/>
       <c r="I4" s="138"/>
       <c r="L4" s="94" t="s">
         <v>489</v>
       </c>
-      <c r="M4" s="178" t="s">
+      <c r="M4" s="184" t="s">
         <v>490</v>
       </c>
-      <c r="N4" s="178"/>
-      <c r="O4" s="178"/>
-      <c r="P4" s="178"/>
-      <c r="Q4" s="178"/>
-      <c r="R4" s="178"/>
-      <c r="S4" s="178"/>
+      <c r="N4" s="184"/>
+      <c r="O4" s="184"/>
+      <c r="P4" s="184"/>
+      <c r="Q4" s="184"/>
+      <c r="R4" s="184"/>
+      <c r="S4" s="184"/>
     </row>
     <row r="5" spans="1:19" ht="16">
       <c r="A5" s="88" t="s">
@@ -27114,13 +27114,13 @@
       </c>
       <c r="H5" s="138"/>
       <c r="I5" s="138"/>
-      <c r="M5" s="178"/>
-      <c r="N5" s="178"/>
-      <c r="O5" s="178"/>
-      <c r="P5" s="178"/>
-      <c r="Q5" s="178"/>
-      <c r="R5" s="178"/>
-      <c r="S5" s="178"/>
+      <c r="M5" s="184"/>
+      <c r="N5" s="184"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="184"/>
+      <c r="R5" s="184"/>
+      <c r="S5" s="184"/>
     </row>
     <row r="6" spans="1:19" ht="16">
       <c r="A6" s="88" t="s">
@@ -27146,13 +27146,13 @@
       </c>
       <c r="H6" s="138"/>
       <c r="I6" s="138"/>
-      <c r="M6" s="178"/>
-      <c r="N6" s="178"/>
-      <c r="O6" s="178"/>
-      <c r="P6" s="178"/>
-      <c r="Q6" s="178"/>
-      <c r="R6" s="178"/>
-      <c r="S6" s="178"/>
+      <c r="M6" s="184"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="184"/>
+      <c r="P6" s="184"/>
+      <c r="Q6" s="184"/>
+      <c r="R6" s="184"/>
+      <c r="S6" s="184"/>
     </row>
     <row r="7" spans="1:19" ht="16">
       <c r="A7" s="88" t="s">
@@ -27178,13 +27178,13 @@
       </c>
       <c r="H7" s="138"/>
       <c r="I7" s="138"/>
-      <c r="M7" s="178"/>
-      <c r="N7" s="178"/>
-      <c r="O7" s="178"/>
-      <c r="P7" s="178"/>
-      <c r="Q7" s="178"/>
-      <c r="R7" s="178"/>
-      <c r="S7" s="178"/>
+      <c r="M7" s="184"/>
+      <c r="N7" s="184"/>
+      <c r="O7" s="184"/>
+      <c r="P7" s="184"/>
+      <c r="Q7" s="184"/>
+      <c r="R7" s="184"/>
+      <c r="S7" s="184"/>
     </row>
     <row r="8" spans="1:19" ht="16">
       <c r="A8" s="88" t="s">
@@ -27210,13 +27210,13 @@
       </c>
       <c r="H8" s="138"/>
       <c r="I8" s="138"/>
-      <c r="M8" s="178"/>
-      <c r="N8" s="178"/>
-      <c r="O8" s="178"/>
-      <c r="P8" s="178"/>
-      <c r="Q8" s="178"/>
-      <c r="R8" s="178"/>
-      <c r="S8" s="178"/>
+      <c r="M8" s="184"/>
+      <c r="N8" s="184"/>
+      <c r="O8" s="184"/>
+      <c r="P8" s="184"/>
+      <c r="Q8" s="184"/>
+      <c r="R8" s="184"/>
+      <c r="S8" s="184"/>
     </row>
     <row r="9" spans="1:19" ht="48">
       <c r="A9" s="88" t="s">
@@ -27242,13 +27242,13 @@
       </c>
       <c r="H9" s="138"/>
       <c r="I9" s="138"/>
-      <c r="M9" s="178"/>
-      <c r="N9" s="178"/>
-      <c r="O9" s="178"/>
-      <c r="P9" s="178"/>
-      <c r="Q9" s="178"/>
-      <c r="R9" s="178"/>
-      <c r="S9" s="178"/>
+      <c r="M9" s="184"/>
+      <c r="N9" s="184"/>
+      <c r="O9" s="184"/>
+      <c r="P9" s="184"/>
+      <c r="Q9" s="184"/>
+      <c r="R9" s="184"/>
+      <c r="S9" s="184"/>
     </row>
     <row r="10" spans="1:19" ht="16">
       <c r="A10" s="90" t="s">
@@ -27274,13 +27274,13 @@
       </c>
       <c r="H10" s="138"/>
       <c r="I10" s="138"/>
-      <c r="M10" s="178"/>
-      <c r="N10" s="178"/>
-      <c r="O10" s="178"/>
-      <c r="P10" s="178"/>
-      <c r="Q10" s="178"/>
-      <c r="R10" s="178"/>
-      <c r="S10" s="178"/>
+      <c r="M10" s="184"/>
+      <c r="N10" s="184"/>
+      <c r="O10" s="184"/>
+      <c r="P10" s="184"/>
+      <c r="Q10" s="184"/>
+      <c r="R10" s="184"/>
+      <c r="S10" s="184"/>
     </row>
     <row r="11" spans="1:19" ht="16">
       <c r="A11" s="92"/>
@@ -27990,11 +27990,11 @@
       <c r="G40" s="34">
         <v>394</v>
       </c>
-      <c r="I40" s="185">
+      <c r="I40" s="179">
         <f>SUM(G41:G42,G51)</f>
         <v>5828</v>
       </c>
-      <c r="J40" s="180">
+      <c r="J40" s="186">
         <v>5867</v>
       </c>
     </row>
@@ -28018,8 +28018,8 @@
       <c r="G41" s="35">
         <v>3404</v>
       </c>
-      <c r="I41" s="186"/>
-      <c r="J41" s="181"/>
+      <c r="I41" s="180"/>
+      <c r="J41" s="187"/>
     </row>
     <row r="42" spans="1:10" ht="16">
       <c r="A42" s="92"/>
@@ -28041,8 +28041,8 @@
       <c r="G42" s="35">
         <v>408</v>
       </c>
-      <c r="I42" s="186"/>
-      <c r="J42" s="181"/>
+      <c r="I42" s="180"/>
+      <c r="J42" s="187"/>
     </row>
     <row r="43" spans="1:10" ht="16">
       <c r="A43" s="92"/>
@@ -28064,8 +28064,8 @@
       <c r="G43" s="35">
         <v>16543</v>
       </c>
-      <c r="I43" s="186"/>
-      <c r="J43" s="181"/>
+      <c r="I43" s="180"/>
+      <c r="J43" s="187"/>
     </row>
     <row r="44" spans="1:10" ht="16">
       <c r="A44" s="92"/>
@@ -28087,11 +28087,11 @@
       <c r="G44" s="35">
         <v>106</v>
       </c>
-      <c r="I44" s="187">
+      <c r="I44" s="181">
         <f>SUM(G43:G46)</f>
         <v>53585</v>
       </c>
-      <c r="J44" s="183">
+      <c r="J44" s="189">
         <v>53593</v>
       </c>
     </row>
@@ -28115,8 +28115,8 @@
       <c r="G45" s="35">
         <v>8568</v>
       </c>
-      <c r="I45" s="187"/>
-      <c r="J45" s="183"/>
+      <c r="I45" s="181"/>
+      <c r="J45" s="189"/>
     </row>
     <row r="46" spans="1:10" ht="32">
       <c r="A46" s="92"/>
@@ -28138,8 +28138,8 @@
       <c r="G46" s="35">
         <v>28368</v>
       </c>
-      <c r="I46" s="187"/>
-      <c r="J46" s="183"/>
+      <c r="I46" s="181"/>
+      <c r="J46" s="189"/>
     </row>
     <row r="47" spans="1:10" ht="16">
       <c r="A47" s="92"/>
@@ -28161,8 +28161,8 @@
       <c r="G47" s="35">
         <v>120</v>
       </c>
-      <c r="I47" s="187"/>
-      <c r="J47" s="183"/>
+      <c r="I47" s="181"/>
+      <c r="J47" s="189"/>
     </row>
     <row r="48" spans="1:10" ht="16">
       <c r="A48" s="92"/>
@@ -28184,11 +28184,11 @@
       <c r="G48" s="35">
         <v>77</v>
       </c>
-      <c r="I48" s="188">
+      <c r="I48" s="182">
         <f>SUM(G52)</f>
         <v>18185</v>
       </c>
-      <c r="J48" s="182">
+      <c r="J48" s="188">
         <v>18101</v>
       </c>
     </row>
@@ -28212,8 +28212,8 @@
       <c r="G49" s="35">
         <v>3160</v>
       </c>
-      <c r="I49" s="188"/>
-      <c r="J49" s="182"/>
+      <c r="I49" s="182"/>
+      <c r="J49" s="188"/>
     </row>
     <row r="50" spans="1:10" ht="16">
       <c r="A50" s="92"/>
@@ -28235,8 +28235,8 @@
       <c r="G50" s="35">
         <v>7278</v>
       </c>
-      <c r="I50" s="188"/>
-      <c r="J50" s="182"/>
+      <c r="I50" s="182"/>
+      <c r="J50" s="188"/>
     </row>
     <row r="51" spans="1:10" ht="32">
       <c r="A51" s="92"/>
@@ -28258,8 +28258,8 @@
       <c r="G51" s="35">
         <v>2016</v>
       </c>
-      <c r="I51" s="188"/>
-      <c r="J51" s="182"/>
+      <c r="I51" s="182"/>
+      <c r="J51" s="188"/>
     </row>
     <row r="52" spans="1:10" ht="16">
       <c r="A52" s="92"/>
@@ -28281,11 +28281,11 @@
       <c r="G52" s="35">
         <v>18185</v>
       </c>
-      <c r="I52" s="189">
+      <c r="I52" s="183">
         <f>SUM(G40,G47:G50,G53:G56)</f>
         <v>15384</v>
       </c>
-      <c r="J52" s="184">
+      <c r="J52" s="178">
         <v>15424</v>
       </c>
     </row>
@@ -28309,8 +28309,8 @@
       <c r="G53" s="35">
         <v>1629</v>
       </c>
-      <c r="I53" s="189"/>
-      <c r="J53" s="184"/>
+      <c r="I53" s="183"/>
+      <c r="J53" s="178"/>
     </row>
     <row r="54" spans="1:10" ht="16">
       <c r="A54" s="92"/>
@@ -28332,8 +28332,8 @@
       <c r="G54" s="35">
         <v>1407</v>
       </c>
-      <c r="I54" s="189"/>
-      <c r="J54" s="184"/>
+      <c r="I54" s="183"/>
+      <c r="J54" s="178"/>
     </row>
     <row r="55" spans="1:10" ht="16">
       <c r="A55" s="91"/>
@@ -28355,8 +28355,8 @@
       <c r="G55" s="36">
         <v>813</v>
       </c>
-      <c r="I55" s="189"/>
-      <c r="J55" s="184"/>
+      <c r="I55" s="183"/>
+      <c r="J55" s="178"/>
     </row>
     <row r="56" spans="1:10" ht="16">
       <c r="A56" s="88" t="s">
@@ -28380,8 +28380,8 @@
       <c r="G56" s="33">
         <v>506</v>
       </c>
-      <c r="I56" s="189"/>
-      <c r="J56" s="184"/>
+      <c r="I56" s="183"/>
+      <c r="J56" s="178"/>
     </row>
     <row r="57" spans="1:10" ht="16">
       <c r="A57" s="92" t="s">
@@ -29499,16 +29499,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="M4:S10"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="J44:J47"/>
     <mergeCell ref="J52:J56"/>
     <mergeCell ref="I40:I43"/>
     <mergeCell ref="I44:I47"/>
     <mergeCell ref="I48:I51"/>
     <mergeCell ref="I52:I56"/>
-    <mergeCell ref="M4:S10"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="J44:J47"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="F2:F1048576">
@@ -35696,10 +35696,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003FD4F6-0596-924C-9C8D-517B5EE2F179}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="B3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -35708,7 +35708,7 @@
     <col min="3" max="6" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:9" ht="16">
       <c r="A1" s="18" t="s">
         <v>1618</v>
       </c>
@@ -35730,8 +35730,12 @@
       <c r="G1" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16">
+      <c r="I1">
+        <f>SUM(G2:G60)</f>
+        <v>316540</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16">
       <c r="A2" t="s">
         <v>1620</v>
       </c>
@@ -35754,7 +35758,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16">
+    <row r="3" spans="1:9" ht="16">
       <c r="A3" t="s">
         <v>1621</v>
       </c>
@@ -35777,7 +35781,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:9" ht="16">
       <c r="A4" t="s">
         <v>1623</v>
       </c>
@@ -35800,7 +35804,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16">
+    <row r="5" spans="1:9" ht="16">
       <c r="A5" t="s">
         <v>1624</v>
       </c>
@@ -35823,7 +35827,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16">
+    <row r="6" spans="1:9" ht="16">
       <c r="A6" t="s">
         <v>1625</v>
       </c>
@@ -35846,7 +35850,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16">
+    <row r="7" spans="1:9" ht="16">
       <c r="A7" t="s">
         <v>1627</v>
       </c>
@@ -35869,7 +35873,7 @@
         <v>6042</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16">
+    <row r="8" spans="1:9" ht="16">
       <c r="A8" t="s">
         <v>1629</v>
       </c>
@@ -35892,7 +35896,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16">
+    <row r="9" spans="1:9" ht="16">
       <c r="A9" t="s">
         <v>1631</v>
       </c>
@@ -35915,7 +35919,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16">
+    <row r="10" spans="1:9" ht="16">
       <c r="A10" t="s">
         <v>1633</v>
       </c>
@@ -35938,7 +35942,7 @@
         <v>30857</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16">
+    <row r="11" spans="1:9" ht="16">
       <c r="A11" t="s">
         <v>1635</v>
       </c>
@@ -35961,7 +35965,7 @@
         <v>4636</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16">
+    <row r="12" spans="1:9" ht="16">
       <c r="A12" t="s">
         <v>1637</v>
       </c>
@@ -35984,7 +35988,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16">
+    <row r="13" spans="1:9" ht="16">
       <c r="A13" t="s">
         <v>1639</v>
       </c>
@@ -36007,7 +36011,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16">
+    <row r="14" spans="1:9" ht="16">
       <c r="A14" t="s">
         <v>1641</v>
       </c>
@@ -36030,7 +36034,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16">
+    <row r="15" spans="1:9" ht="16">
       <c r="A15" t="s">
         <v>1643</v>
       </c>
@@ -36053,7 +36057,7 @@
         <v>5520</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16">
+    <row r="16" spans="1:9" ht="16">
       <c r="A16" t="s">
         <v>1645</v>
       </c>
@@ -44225,10 +44229,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6088356-EAF0-3047-99CA-B8AF6FB8D417}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="179" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -44282,7 +44286,7 @@
         <v>2377549</v>
       </c>
       <c r="D3" s="120">
-        <f t="shared" ref="D3:D17" si="0">(B3/C3)*100000</f>
+        <f t="shared" ref="D3:D19" si="0">(B3/C3)*100000</f>
         <v>1362.7479391591928</v>
       </c>
     </row>
@@ -44524,6 +44528,30 @@
       </c>
       <c r="E17" t="s">
         <v>1605</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>2019</v>
+      </c>
+      <c r="D18" s="120" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>2020</v>
+      </c>
+      <c r="B19">
+        <v>316540</v>
+      </c>
+      <c r="C19" s="120">
+        <v>39512223</v>
+      </c>
+      <c r="D19" s="120">
+        <f t="shared" si="0"/>
+        <v>801.11918785232604</v>
       </c>
     </row>
   </sheetData>
@@ -62222,8 +62250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DCE92E-083B-BD4D-9E79-C8655C97D55B}">
   <dimension ref="A1:I284"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>

</xml_diff>

<commit_message>
Added population data for 2019.
</commit_message>
<xml_diff>
--- a/CA 1900-2020 Project.xlsx
+++ b/CA 1900-2020 Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AA5C6A-BBB5-6C4D-B660-FDAC112F6FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654803E6-F4FD-1C4A-8798-5C53B48D288E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="6" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y1900" sheetId="1" r:id="rId1"/>
@@ -6136,6 +6136,24 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6152,24 +6170,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -27052,7 +27052,7 @@
       <c r="G3" s="34">
         <v>85</v>
       </c>
-      <c r="H3" s="185"/>
+      <c r="H3" s="179"/>
       <c r="I3" s="138"/>
     </row>
     <row r="4" spans="1:19" ht="16" customHeight="1">
@@ -27075,20 +27075,20 @@
       <c r="G4" s="36">
         <v>19</v>
       </c>
-      <c r="H4" s="185"/>
+      <c r="H4" s="179"/>
       <c r="I4" s="138"/>
       <c r="L4" s="94" t="s">
         <v>489</v>
       </c>
-      <c r="M4" s="184" t="s">
+      <c r="M4" s="178" t="s">
         <v>490</v>
       </c>
-      <c r="N4" s="184"/>
-      <c r="O4" s="184"/>
-      <c r="P4" s="184"/>
-      <c r="Q4" s="184"/>
-      <c r="R4" s="184"/>
-      <c r="S4" s="184"/>
+      <c r="N4" s="178"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="178"/>
+      <c r="Q4" s="178"/>
+      <c r="R4" s="178"/>
+      <c r="S4" s="178"/>
     </row>
     <row r="5" spans="1:19" ht="16">
       <c r="A5" s="88" t="s">
@@ -27114,13 +27114,13 @@
       </c>
       <c r="H5" s="138"/>
       <c r="I5" s="138"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
-      <c r="O5" s="184"/>
-      <c r="P5" s="184"/>
-      <c r="Q5" s="184"/>
-      <c r="R5" s="184"/>
-      <c r="S5" s="184"/>
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
+      <c r="O5" s="178"/>
+      <c r="P5" s="178"/>
+      <c r="Q5" s="178"/>
+      <c r="R5" s="178"/>
+      <c r="S5" s="178"/>
     </row>
     <row r="6" spans="1:19" ht="16">
       <c r="A6" s="88" t="s">
@@ -27146,13 +27146,13 @@
       </c>
       <c r="H6" s="138"/>
       <c r="I6" s="138"/>
-      <c r="M6" s="184"/>
-      <c r="N6" s="184"/>
-      <c r="O6" s="184"/>
-      <c r="P6" s="184"/>
-      <c r="Q6" s="184"/>
-      <c r="R6" s="184"/>
-      <c r="S6" s="184"/>
+      <c r="M6" s="178"/>
+      <c r="N6" s="178"/>
+      <c r="O6" s="178"/>
+      <c r="P6" s="178"/>
+      <c r="Q6" s="178"/>
+      <c r="R6" s="178"/>
+      <c r="S6" s="178"/>
     </row>
     <row r="7" spans="1:19" ht="16">
       <c r="A7" s="88" t="s">
@@ -27178,13 +27178,13 @@
       </c>
       <c r="H7" s="138"/>
       <c r="I7" s="138"/>
-      <c r="M7" s="184"/>
-      <c r="N7" s="184"/>
-      <c r="O7" s="184"/>
-      <c r="P7" s="184"/>
-      <c r="Q7" s="184"/>
-      <c r="R7" s="184"/>
-      <c r="S7" s="184"/>
+      <c r="M7" s="178"/>
+      <c r="N7" s="178"/>
+      <c r="O7" s="178"/>
+      <c r="P7" s="178"/>
+      <c r="Q7" s="178"/>
+      <c r="R7" s="178"/>
+      <c r="S7" s="178"/>
     </row>
     <row r="8" spans="1:19" ht="16">
       <c r="A8" s="88" t="s">
@@ -27210,13 +27210,13 @@
       </c>
       <c r="H8" s="138"/>
       <c r="I8" s="138"/>
-      <c r="M8" s="184"/>
-      <c r="N8" s="184"/>
-      <c r="O8" s="184"/>
-      <c r="P8" s="184"/>
-      <c r="Q8" s="184"/>
-      <c r="R8" s="184"/>
-      <c r="S8" s="184"/>
+      <c r="M8" s="178"/>
+      <c r="N8" s="178"/>
+      <c r="O8" s="178"/>
+      <c r="P8" s="178"/>
+      <c r="Q8" s="178"/>
+      <c r="R8" s="178"/>
+      <c r="S8" s="178"/>
     </row>
     <row r="9" spans="1:19" ht="48">
       <c r="A9" s="88" t="s">
@@ -27242,13 +27242,13 @@
       </c>
       <c r="H9" s="138"/>
       <c r="I9" s="138"/>
-      <c r="M9" s="184"/>
-      <c r="N9" s="184"/>
-      <c r="O9" s="184"/>
-      <c r="P9" s="184"/>
-      <c r="Q9" s="184"/>
-      <c r="R9" s="184"/>
-      <c r="S9" s="184"/>
+      <c r="M9" s="178"/>
+      <c r="N9" s="178"/>
+      <c r="O9" s="178"/>
+      <c r="P9" s="178"/>
+      <c r="Q9" s="178"/>
+      <c r="R9" s="178"/>
+      <c r="S9" s="178"/>
     </row>
     <row r="10" spans="1:19" ht="16">
       <c r="A10" s="90" t="s">
@@ -27274,13 +27274,13 @@
       </c>
       <c r="H10" s="138"/>
       <c r="I10" s="138"/>
-      <c r="M10" s="184"/>
-      <c r="N10" s="184"/>
-      <c r="O10" s="184"/>
-      <c r="P10" s="184"/>
-      <c r="Q10" s="184"/>
-      <c r="R10" s="184"/>
-      <c r="S10" s="184"/>
+      <c r="M10" s="178"/>
+      <c r="N10" s="178"/>
+      <c r="O10" s="178"/>
+      <c r="P10" s="178"/>
+      <c r="Q10" s="178"/>
+      <c r="R10" s="178"/>
+      <c r="S10" s="178"/>
     </row>
     <row r="11" spans="1:19" ht="16">
       <c r="A11" s="92"/>
@@ -27990,11 +27990,11 @@
       <c r="G40" s="34">
         <v>394</v>
       </c>
-      <c r="I40" s="179">
+      <c r="I40" s="185">
         <f>SUM(G41:G42,G51)</f>
         <v>5828</v>
       </c>
-      <c r="J40" s="186">
+      <c r="J40" s="180">
         <v>5867</v>
       </c>
     </row>
@@ -28018,8 +28018,8 @@
       <c r="G41" s="35">
         <v>3404</v>
       </c>
-      <c r="I41" s="180"/>
-      <c r="J41" s="187"/>
+      <c r="I41" s="186"/>
+      <c r="J41" s="181"/>
     </row>
     <row r="42" spans="1:10" ht="16">
       <c r="A42" s="92"/>
@@ -28041,8 +28041,8 @@
       <c r="G42" s="35">
         <v>408</v>
       </c>
-      <c r="I42" s="180"/>
-      <c r="J42" s="187"/>
+      <c r="I42" s="186"/>
+      <c r="J42" s="181"/>
     </row>
     <row r="43" spans="1:10" ht="16">
       <c r="A43" s="92"/>
@@ -28064,8 +28064,8 @@
       <c r="G43" s="35">
         <v>16543</v>
       </c>
-      <c r="I43" s="180"/>
-      <c r="J43" s="187"/>
+      <c r="I43" s="186"/>
+      <c r="J43" s="181"/>
     </row>
     <row r="44" spans="1:10" ht="16">
       <c r="A44" s="92"/>
@@ -28087,11 +28087,11 @@
       <c r="G44" s="35">
         <v>106</v>
       </c>
-      <c r="I44" s="181">
+      <c r="I44" s="187">
         <f>SUM(G43:G46)</f>
         <v>53585</v>
       </c>
-      <c r="J44" s="189">
+      <c r="J44" s="183">
         <v>53593</v>
       </c>
     </row>
@@ -28115,8 +28115,8 @@
       <c r="G45" s="35">
         <v>8568</v>
       </c>
-      <c r="I45" s="181"/>
-      <c r="J45" s="189"/>
+      <c r="I45" s="187"/>
+      <c r="J45" s="183"/>
     </row>
     <row r="46" spans="1:10" ht="32">
       <c r="A46" s="92"/>
@@ -28138,8 +28138,8 @@
       <c r="G46" s="35">
         <v>28368</v>
       </c>
-      <c r="I46" s="181"/>
-      <c r="J46" s="189"/>
+      <c r="I46" s="187"/>
+      <c r="J46" s="183"/>
     </row>
     <row r="47" spans="1:10" ht="16">
       <c r="A47" s="92"/>
@@ -28161,8 +28161,8 @@
       <c r="G47" s="35">
         <v>120</v>
       </c>
-      <c r="I47" s="181"/>
-      <c r="J47" s="189"/>
+      <c r="I47" s="187"/>
+      <c r="J47" s="183"/>
     </row>
     <row r="48" spans="1:10" ht="16">
       <c r="A48" s="92"/>
@@ -28184,11 +28184,11 @@
       <c r="G48" s="35">
         <v>77</v>
       </c>
-      <c r="I48" s="182">
+      <c r="I48" s="188">
         <f>SUM(G52)</f>
         <v>18185</v>
       </c>
-      <c r="J48" s="188">
+      <c r="J48" s="182">
         <v>18101</v>
       </c>
     </row>
@@ -28212,8 +28212,8 @@
       <c r="G49" s="35">
         <v>3160</v>
       </c>
-      <c r="I49" s="182"/>
-      <c r="J49" s="188"/>
+      <c r="I49" s="188"/>
+      <c r="J49" s="182"/>
     </row>
     <row r="50" spans="1:10" ht="16">
       <c r="A50" s="92"/>
@@ -28235,8 +28235,8 @@
       <c r="G50" s="35">
         <v>7278</v>
       </c>
-      <c r="I50" s="182"/>
-      <c r="J50" s="188"/>
+      <c r="I50" s="188"/>
+      <c r="J50" s="182"/>
     </row>
     <row r="51" spans="1:10" ht="32">
       <c r="A51" s="92"/>
@@ -28258,8 +28258,8 @@
       <c r="G51" s="35">
         <v>2016</v>
       </c>
-      <c r="I51" s="182"/>
-      <c r="J51" s="188"/>
+      <c r="I51" s="188"/>
+      <c r="J51" s="182"/>
     </row>
     <row r="52" spans="1:10" ht="16">
       <c r="A52" s="92"/>
@@ -28281,11 +28281,11 @@
       <c r="G52" s="35">
         <v>18185</v>
       </c>
-      <c r="I52" s="183">
+      <c r="I52" s="189">
         <f>SUM(G40,G47:G50,G53:G56)</f>
         <v>15384</v>
       </c>
-      <c r="J52" s="178">
+      <c r="J52" s="184">
         <v>15424</v>
       </c>
     </row>
@@ -28309,8 +28309,8 @@
       <c r="G53" s="35">
         <v>1629</v>
       </c>
-      <c r="I53" s="183"/>
-      <c r="J53" s="178"/>
+      <c r="I53" s="189"/>
+      <c r="J53" s="184"/>
     </row>
     <row r="54" spans="1:10" ht="16">
       <c r="A54" s="92"/>
@@ -28332,8 +28332,8 @@
       <c r="G54" s="35">
         <v>1407</v>
       </c>
-      <c r="I54" s="183"/>
-      <c r="J54" s="178"/>
+      <c r="I54" s="189"/>
+      <c r="J54" s="184"/>
     </row>
     <row r="55" spans="1:10" ht="16">
       <c r="A55" s="91"/>
@@ -28355,8 +28355,8 @@
       <c r="G55" s="36">
         <v>813</v>
       </c>
-      <c r="I55" s="183"/>
-      <c r="J55" s="178"/>
+      <c r="I55" s="189"/>
+      <c r="J55" s="184"/>
     </row>
     <row r="56" spans="1:10" ht="16">
       <c r="A56" s="88" t="s">
@@ -28380,8 +28380,8 @@
       <c r="G56" s="33">
         <v>506</v>
       </c>
-      <c r="I56" s="183"/>
-      <c r="J56" s="178"/>
+      <c r="I56" s="189"/>
+      <c r="J56" s="184"/>
     </row>
     <row r="57" spans="1:10" ht="16">
       <c r="A57" s="92" t="s">
@@ -29499,16 +29499,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J52:J56"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="I52:I56"/>
     <mergeCell ref="M4:S10"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="J40:J43"/>
     <mergeCell ref="J48:J51"/>
     <mergeCell ref="J44:J47"/>
-    <mergeCell ref="J52:J56"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="I52:I56"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="F2:F1048576">
@@ -29558,7 +29558,7 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
@@ -34258,11 +34258,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE00D5B-D363-6A46-AEA9-149824DE4DAC}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -34271,7 +34271,7 @@
     <col min="3" max="6" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:9" ht="16">
       <c r="A1" s="18" t="s">
         <v>1618</v>
       </c>
@@ -34293,8 +34293,12 @@
       <c r="G1" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16">
+      <c r="I1">
+        <f>SUM(G2:G60)</f>
+        <v>267031</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16">
       <c r="A2" t="s">
         <v>1620</v>
       </c>
@@ -34317,7 +34321,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16">
+    <row r="3" spans="1:9" ht="16">
       <c r="A3" t="s">
         <v>1621</v>
       </c>
@@ -34340,7 +34344,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:9" ht="16">
       <c r="A4" t="s">
         <v>1623</v>
       </c>
@@ -34363,7 +34367,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16">
+    <row r="5" spans="1:9" ht="16">
       <c r="A5" t="s">
         <v>1624</v>
       </c>
@@ -34386,7 +34390,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16">
+    <row r="6" spans="1:9" ht="16">
       <c r="A6" t="s">
         <v>1625</v>
       </c>
@@ -34409,7 +34413,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16">
+    <row r="7" spans="1:9" ht="16">
       <c r="A7" t="s">
         <v>1627</v>
       </c>
@@ -34432,7 +34436,7 @@
         <v>5654</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16">
+    <row r="8" spans="1:9" ht="16">
       <c r="A8" t="s">
         <v>1629</v>
       </c>
@@ -34455,7 +34459,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16">
+    <row r="9" spans="1:9" ht="16">
       <c r="A9" t="s">
         <v>1631</v>
       </c>
@@ -34478,7 +34482,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16">
+    <row r="10" spans="1:9" ht="16">
       <c r="A10" t="s">
         <v>1633</v>
       </c>
@@ -34501,7 +34505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16">
+    <row r="11" spans="1:9" ht="16">
       <c r="A11" t="s">
         <v>1635</v>
       </c>
@@ -34524,7 +34528,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16">
+    <row r="12" spans="1:9" ht="16">
       <c r="A12" t="s">
         <v>1637</v>
       </c>
@@ -34547,7 +34551,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16">
+    <row r="13" spans="1:9" ht="16">
       <c r="A13" t="s">
         <v>1639</v>
       </c>
@@ -34570,7 +34574,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16">
+    <row r="14" spans="1:9" ht="16">
       <c r="A14" t="s">
         <v>1641</v>
       </c>
@@ -34593,7 +34597,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16">
+    <row r="15" spans="1:9" ht="16">
       <c r="A15" t="s">
         <v>1643</v>
       </c>
@@ -34616,7 +34620,7 @@
         <v>5497</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16">
+    <row r="16" spans="1:9" ht="16">
       <c r="A16" t="s">
         <v>1645</v>
       </c>
@@ -35698,8 +35702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003FD4F6-0596-924C-9C8D-517B5EE2F179}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -44231,8 +44236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6088356-EAF0-3047-99CA-B8AF6FB8D417}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="179" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -44534,24 +44539,30 @@
       <c r="A18">
         <v>2019</v>
       </c>
-      <c r="D18" s="120" t="e">
+      <c r="B18" s="120">
+        <v>267031</v>
+      </c>
+      <c r="C18" s="120">
+        <v>39512223</v>
+      </c>
+      <c r="D18" s="120">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>675.81872070321128</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
         <v>2020</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="120">
         <v>316540</v>
       </c>
       <c r="C19" s="120">
-        <v>39512223</v>
+        <v>39538223</v>
       </c>
       <c r="D19" s="120">
         <f t="shared" si="0"/>
-        <v>801.11918785232604</v>
+        <v>800.59237867114064</v>
       </c>
     </row>
   </sheetData>
@@ -62250,7 +62261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DCE92E-083B-BD4D-9E79-C8655C97D55B}">
   <dimension ref="A1:I284"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>

</xml_diff>